<commit_message>
Remove end activity from data
</commit_message>
<xml_diff>
--- a/data/Case study 1.xlsx
+++ b/data/Case study 1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B2B807-468F-4FA6-A469-24571B2E9FA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08AA6D8-4EC2-4316-9938-B1216461EE46}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -453,7 +453,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -635,22 +635,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -679,10 +709,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -721,15 +747,7 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -803,13 +821,46 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -819,10 +870,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -858,10 +905,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -870,39 +913,66 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -1188,2489 +1258,2495 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC8281"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="5" customWidth="1"/>
-    <col min="8" max="8" width="42" style="5" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="5"/>
-    <col min="10" max="10" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="17.140625" style="5" customWidth="1"/>
-    <col min="18" max="18" width="40.28515625" style="5" customWidth="1"/>
-    <col min="19" max="21" width="9.140625" style="5"/>
-    <col min="22" max="22" width="44.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="28.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="30" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="42" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="2"/>
+    <col min="10" max="10" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="17.140625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="40.28515625" style="2" customWidth="1"/>
+    <col min="19" max="21" width="9.140625" style="2"/>
+    <col min="22" max="22" width="44.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="28.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2">
+      <c r="A1" s="69">
         <v>1</v>
       </c>
-      <c r="B1" s="3">
+      <c r="B1" s="70">
         <v>2</v>
       </c>
-      <c r="C1" s="3">
+      <c r="C1" s="70">
         <v>3</v>
       </c>
-      <c r="D1" s="3">
+      <c r="D1" s="70">
         <v>4</v>
       </c>
-      <c r="E1" s="3">
+      <c r="E1" s="70">
         <v>5</v>
       </c>
-      <c r="F1" s="4">
+      <c r="F1" s="71">
         <v>6</v>
       </c>
-      <c r="G1" s="5">
+      <c r="G1" s="2">
         <v>7</v>
       </c>
-      <c r="H1" s="5">
+      <c r="H1" s="2">
         <v>8</v>
       </c>
-      <c r="I1" s="5">
+      <c r="I1" s="2">
         <v>9</v>
       </c>
-      <c r="J1" s="5">
+      <c r="J1" s="2">
         <v>10</v>
       </c>
-      <c r="K1" s="5">
+      <c r="K1" s="2">
         <v>11</v>
       </c>
-      <c r="L1" s="5">
+      <c r="L1" s="2">
         <v>12</v>
       </c>
-      <c r="M1" s="5">
+      <c r="M1" s="2">
         <v>13</v>
       </c>
-      <c r="N1" s="5">
+      <c r="N1" s="2">
         <v>14</v>
       </c>
-      <c r="O1" s="5">
+      <c r="O1" s="2">
         <v>15</v>
       </c>
-      <c r="P1" s="5">
+      <c r="P1" s="2">
         <v>16</v>
       </c>
-      <c r="Q1" s="5">
+      <c r="Q1" s="2">
         <v>17</v>
       </c>
-      <c r="R1" s="5">
+      <c r="R1" s="2">
         <v>18</v>
       </c>
-      <c r="S1" s="5">
+      <c r="S1" s="2">
         <v>19</v>
       </c>
-      <c r="T1" s="5">
+      <c r="T1" s="2">
         <v>20</v>
       </c>
-      <c r="U1" s="5">
+      <c r="U1" s="2">
         <v>21</v>
       </c>
-      <c r="V1" s="5">
+      <c r="V1" s="2">
         <v>22</v>
       </c>
-      <c r="W1" s="5">
+      <c r="W1" s="2">
         <v>23</v>
       </c>
-      <c r="X1" s="5">
+      <c r="X1" s="2">
         <v>24</v>
       </c>
-      <c r="Y1" s="5">
+      <c r="Y1" s="2">
         <v>25</v>
       </c>
-      <c r="Z1" s="5">
+      <c r="Z1" s="2">
         <v>26</v>
       </c>
-      <c r="AA1" s="5">
+      <c r="AA1" s="2">
         <v>27</v>
       </c>
-      <c r="AB1" s="5">
+      <c r="AB1" s="2">
         <v>28</v>
       </c>
-      <c r="AC1" s="5">
+      <c r="AC1" s="2">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="72" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="73" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="62" t="s">
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="H2" s="57" t="s">
+      <c r="H2" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="I2" s="52" t="s">
+      <c r="I2" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52" t="s">
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="50" t="s">
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="52" t="s">
         <v>8</v>
       </c>
       <c r="Q2" s="63" t="s">
         <v>96</v>
       </c>
-      <c r="R2" s="54" t="s">
+      <c r="R2" s="55" t="s">
         <v>95</v>
       </c>
-      <c r="S2" s="53" t="s">
+      <c r="S2" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
-      <c r="V2" s="53" t="s">
+      <c r="T2" s="48"/>
+      <c r="U2" s="48"/>
+      <c r="V2" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="W2" s="72" t="s">
+      <c r="W2" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="X2" s="65" t="s">
+      <c r="X2" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="Y2" s="67" t="s">
+      <c r="Y2" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="Z2" s="69" t="s">
+      <c r="Z2" s="47" t="s">
         <v>102</v>
       </c>
-      <c r="AA2" s="69"/>
-      <c r="AB2" s="69"/>
-      <c r="AC2" s="69" t="s">
+      <c r="AA2" s="47"/>
+      <c r="AB2" s="47"/>
+      <c r="AC2" s="78" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="56"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="6" t="s">
+      <c r="A3" s="57"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="62"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="7" t="s">
+      <c r="F3" s="75"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="N3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="P3" s="51"/>
+      <c r="P3" s="53"/>
       <c r="Q3" s="64"/>
-      <c r="R3" s="55"/>
-      <c r="S3" s="8" t="s">
+      <c r="R3" s="56"/>
+      <c r="S3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="T3" s="8" t="s">
+      <c r="T3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="U3" s="8" t="s">
+      <c r="U3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="V3" s="71"/>
-      <c r="W3" s="73"/>
-      <c r="X3" s="66"/>
-      <c r="Y3" s="68"/>
-      <c r="Z3" s="9" t="s">
+      <c r="V3" s="49"/>
+      <c r="W3" s="51"/>
+      <c r="X3" s="44"/>
+      <c r="Y3" s="46"/>
+      <c r="Z3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="AA3" s="9" t="s">
+      <c r="AA3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="AB3" s="9" t="s">
+      <c r="AB3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="AC3" s="70"/>
+      <c r="AC3" s="79"/>
     </row>
     <row r="4" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
+      <c r="A4" s="7">
         <v>1</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="9">
         <v>0</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="10">
         <v>0</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="9">
         <v>0</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="15">
+      <c r="F4" s="76"/>
+      <c r="G4" s="11">
         <v>1</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="9">
         <v>51</v>
       </c>
-      <c r="J4" s="17">
+      <c r="J4" s="13">
         <v>52</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="9">
         <v>52</v>
       </c>
-      <c r="L4" s="18">
+      <c r="L4" s="14">
         <v>0.5</v>
       </c>
-      <c r="M4" s="48">
+      <c r="M4" s="41">
         <f>N4*(1-(L4*(J4-I4)/J4))</f>
         <v>118846.15384615384</v>
       </c>
-      <c r="N4" s="19">
+      <c r="N4" s="15">
         <v>120000</v>
       </c>
-      <c r="O4" s="48">
+      <c r="O4" s="41">
         <f>N4*(1-(L4*(J4-K4)/J4))</f>
         <v>120000</v>
       </c>
-      <c r="P4" s="20">
+      <c r="P4" s="16">
         <v>3</v>
       </c>
-      <c r="Q4" s="21">
+      <c r="Q4" s="17">
         <v>1</v>
       </c>
-      <c r="R4" s="22" t="s">
+      <c r="R4" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="S4" s="18">
+      <c r="S4" s="14">
         <v>96</v>
       </c>
-      <c r="T4" s="22">
+      <c r="T4" s="18">
         <v>105</v>
       </c>
-      <c r="U4" s="18">
+      <c r="U4" s="14">
         <v>119</v>
       </c>
-      <c r="V4" s="18">
+      <c r="V4" s="14">
         <v>3</v>
       </c>
-      <c r="W4" s="23">
+      <c r="W4" s="19">
         <v>0.2</v>
       </c>
-      <c r="X4" s="24">
+      <c r="X4" s="20">
         <v>1</v>
       </c>
-      <c r="Y4" s="16"/>
-      <c r="Z4" s="12">
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="9">
         <v>120</v>
       </c>
-      <c r="AA4" s="16">
+      <c r="AA4" s="12">
         <v>121</v>
       </c>
-      <c r="AB4" s="12">
+      <c r="AB4" s="9">
         <v>154</v>
       </c>
-      <c r="AC4" s="12" t="s">
+      <c r="AC4" s="80" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
+      <c r="A5" s="7">
         <v>2</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="9">
         <v>0</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="10">
         <v>0</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="9">
         <v>0</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="15">
+      <c r="F5" s="76"/>
+      <c r="G5" s="11">
         <v>2</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="9">
         <v>7</v>
       </c>
-      <c r="J5" s="17">
+      <c r="J5" s="13">
         <v>7</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="9">
         <v>7</v>
       </c>
-      <c r="L5" s="18">
+      <c r="L5" s="14">
         <v>0.5</v>
       </c>
-      <c r="M5" s="48">
+      <c r="M5" s="41">
         <f t="shared" ref="M5:M22" si="0">N5*(1-(L5*(J5-I5)/J5))</f>
         <v>30000</v>
       </c>
-      <c r="N5" s="19">
+      <c r="N5" s="15">
         <v>30000</v>
       </c>
-      <c r="O5" s="48">
+      <c r="O5" s="41">
         <f t="shared" ref="O5:O22" si="1">N5*(1-(L5*(J5-K5)/J5))</f>
         <v>30000</v>
       </c>
-      <c r="P5" s="20">
+      <c r="P5" s="16">
         <v>4</v>
       </c>
-      <c r="Q5" s="21">
+      <c r="Q5" s="17">
         <v>2</v>
       </c>
-      <c r="R5" s="22" t="s">
+      <c r="R5" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="S5" s="18">
+      <c r="S5" s="14">
         <v>13</v>
       </c>
-      <c r="T5" s="22">
+      <c r="T5" s="18">
         <v>14</v>
       </c>
-      <c r="U5" s="18">
+      <c r="U5" s="14">
         <v>15</v>
       </c>
-      <c r="V5" s="18">
+      <c r="V5" s="14">
         <v>4</v>
       </c>
-      <c r="W5" s="23">
+      <c r="W5" s="19">
         <v>0.05</v>
       </c>
-      <c r="X5" s="24">
+      <c r="X5" s="20">
         <v>2</v>
       </c>
-      <c r="Y5" s="16"/>
-      <c r="Z5" s="12">
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="9">
         <v>180</v>
       </c>
-      <c r="AA5" s="16">
+      <c r="AA5" s="12">
         <v>190</v>
       </c>
-      <c r="AB5" s="12">
+      <c r="AB5" s="9">
         <v>240</v>
       </c>
-      <c r="AC5" s="12" t="s">
+      <c r="AC5" s="80" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+      <c r="A6" s="7">
         <v>3</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="9">
         <v>865</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="10">
         <v>920</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="9">
         <v>1040</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="32">
         <v>1</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="11">
         <v>3</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H6" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="9">
         <v>53</v>
       </c>
-      <c r="J6" s="17">
+      <c r="J6" s="13">
         <v>65</v>
       </c>
-      <c r="K6" s="12">
+      <c r="K6" s="9">
         <v>65</v>
       </c>
-      <c r="L6" s="18">
+      <c r="L6" s="14">
         <v>0.5</v>
       </c>
-      <c r="M6" s="48">
+      <c r="M6" s="41">
         <f t="shared" si="0"/>
         <v>136153.84615384616</v>
       </c>
-      <c r="N6" s="19">
+      <c r="N6" s="15">
         <v>150000</v>
       </c>
-      <c r="O6" s="48">
+      <c r="O6" s="41">
         <f t="shared" si="1"/>
         <v>150000</v>
       </c>
-      <c r="P6" s="20">
+      <c r="P6" s="16">
         <v>7</v>
       </c>
-      <c r="Q6" s="21">
+      <c r="Q6" s="17">
         <v>3</v>
       </c>
-      <c r="R6" s="22" t="s">
+      <c r="R6" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="S6" s="18">
+      <c r="S6" s="14">
         <v>63</v>
       </c>
-      <c r="T6" s="22">
+      <c r="T6" s="18">
         <v>70</v>
       </c>
-      <c r="U6" s="18">
+      <c r="U6" s="14">
         <v>78</v>
       </c>
-      <c r="V6" s="18">
+      <c r="V6" s="14">
         <v>7</v>
       </c>
-      <c r="W6" s="23">
+      <c r="W6" s="19">
         <v>0.15</v>
       </c>
-      <c r="X6" s="24">
+      <c r="X6" s="20">
         <v>3</v>
       </c>
-      <c r="Y6" s="16"/>
-      <c r="Z6" s="12">
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="9">
         <v>225</v>
       </c>
-      <c r="AA6" s="16">
+      <c r="AA6" s="12">
         <v>250</v>
       </c>
-      <c r="AB6" s="12">
+      <c r="AB6" s="9">
         <v>310</v>
       </c>
-      <c r="AC6" s="12" t="s">
+      <c r="AC6" s="80" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+      <c r="A7" s="7">
         <v>4</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="9">
         <v>128</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="10">
         <v>130</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="9">
         <v>164</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="32">
         <v>1</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="11">
         <v>4</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="H7" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="9">
         <v>22</v>
       </c>
-      <c r="J7" s="17">
+      <c r="J7" s="13">
         <v>26</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="9">
         <v>29</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="14">
         <v>0.5</v>
       </c>
-      <c r="M7" s="48">
+      <c r="M7" s="41">
         <f t="shared" si="0"/>
         <v>44307.692307692312</v>
       </c>
-      <c r="N7" s="19">
+      <c r="N7" s="15">
         <v>48000</v>
       </c>
-      <c r="O7" s="48">
+      <c r="O7" s="41">
         <f t="shared" si="1"/>
         <v>50769.230769230773</v>
       </c>
-      <c r="P7" s="20">
+      <c r="P7" s="16">
         <v>8</v>
       </c>
-      <c r="Q7" s="21">
+      <c r="Q7" s="17">
         <v>4</v>
       </c>
-      <c r="R7" s="22" t="s">
+      <c r="R7" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="S7" s="18">
+      <c r="S7" s="14">
         <v>35</v>
       </c>
-      <c r="T7" s="22">
+      <c r="T7" s="18">
         <v>35</v>
       </c>
-      <c r="U7" s="18">
+      <c r="U7" s="14">
         <v>41</v>
       </c>
-      <c r="V7" s="18">
+      <c r="V7" s="14">
         <v>8</v>
       </c>
-      <c r="W7" s="23">
+      <c r="W7" s="19">
         <v>0.2</v>
       </c>
-      <c r="X7" s="24">
+      <c r="X7" s="20">
         <v>4</v>
       </c>
-      <c r="Y7" s="16"/>
-      <c r="Z7" s="12">
+      <c r="Y7" s="12"/>
+      <c r="Z7" s="9">
         <v>148</v>
       </c>
-      <c r="AA7" s="16">
+      <c r="AA7" s="12">
         <v>155</v>
       </c>
-      <c r="AB7" s="12">
+      <c r="AB7" s="9">
         <v>170</v>
       </c>
-      <c r="AC7" s="12" t="s">
+      <c r="AC7" s="80" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+      <c r="A8" s="7">
         <v>5</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="9">
         <v>0</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="10">
         <v>0</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="9">
         <v>0</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="11">
         <v>5</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="9">
         <v>21</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8" s="13">
         <v>26</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K8" s="9">
         <v>26</v>
       </c>
-      <c r="L8" s="18">
+      <c r="L8" s="14">
         <v>0.5</v>
       </c>
-      <c r="M8" s="48">
+      <c r="M8" s="41">
         <f t="shared" si="0"/>
         <v>677884.61538461538</v>
       </c>
-      <c r="N8" s="19">
+      <c r="N8" s="15">
         <v>750000</v>
       </c>
-      <c r="O8" s="48">
+      <c r="O8" s="41">
         <f t="shared" si="1"/>
         <v>750000</v>
       </c>
-      <c r="P8" s="20">
+      <c r="P8" s="16">
         <v>9</v>
       </c>
-      <c r="Q8" s="21">
+      <c r="Q8" s="17">
         <v>5</v>
       </c>
-      <c r="R8" s="22" t="s">
+      <c r="R8" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="S8" s="18">
+      <c r="S8" s="14">
         <v>34</v>
       </c>
-      <c r="T8" s="22">
+      <c r="T8" s="18">
         <v>35</v>
       </c>
-      <c r="U8" s="18">
+      <c r="U8" s="14">
         <v>40</v>
       </c>
-      <c r="V8" s="18">
+      <c r="V8" s="14">
         <v>9</v>
       </c>
-      <c r="W8" s="23">
+      <c r="W8" s="19">
         <v>0.1</v>
       </c>
-      <c r="X8" s="24"/>
-      <c r="Y8" s="16"/>
-      <c r="Z8" s="12"/>
-      <c r="AA8" s="16"/>
-      <c r="AB8" s="12"/>
-      <c r="AC8" s="12"/>
+      <c r="X8" s="20"/>
+      <c r="Y8" s="12"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="12"/>
+      <c r="AB8" s="9"/>
+      <c r="AC8" s="80"/>
     </row>
     <row r="9" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+      <c r="A9" s="7">
         <v>6</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="9">
         <v>0</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="10">
         <v>0</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="9">
         <v>0</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="32">
         <v>5</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="11">
         <v>6</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="9">
         <v>47</v>
       </c>
-      <c r="J9" s="17">
+      <c r="J9" s="13">
         <v>52</v>
       </c>
-      <c r="K9" s="12">
+      <c r="K9" s="9">
         <v>55</v>
       </c>
-      <c r="L9" s="18">
+      <c r="L9" s="14">
         <v>0.5</v>
       </c>
-      <c r="M9" s="48">
+      <c r="M9" s="41">
         <f t="shared" si="0"/>
         <v>190384.61538461538</v>
       </c>
-      <c r="N9" s="19">
+      <c r="N9" s="15">
         <v>200000</v>
       </c>
-      <c r="O9" s="48">
+      <c r="O9" s="41">
         <f t="shared" si="1"/>
         <v>205769.23076923075</v>
       </c>
-      <c r="P9" s="20">
+      <c r="P9" s="16">
         <v>10</v>
       </c>
-      <c r="Q9" s="21">
+      <c r="Q9" s="17">
         <v>6</v>
       </c>
-      <c r="R9" s="22" t="s">
+      <c r="R9" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="S9" s="18">
+      <c r="S9" s="14">
         <v>14</v>
       </c>
-      <c r="T9" s="22">
+      <c r="T9" s="18">
         <v>14</v>
       </c>
-      <c r="U9" s="18">
+      <c r="U9" s="14">
         <v>15</v>
       </c>
-      <c r="V9" s="18">
+      <c r="V9" s="14">
         <v>10</v>
       </c>
-      <c r="W9" s="23">
+      <c r="W9" s="19">
         <v>0.1</v>
       </c>
-      <c r="X9" s="24"/>
-      <c r="Y9" s="16"/>
-      <c r="Z9" s="12"/>
-      <c r="AA9" s="16"/>
-      <c r="AB9" s="12"/>
-      <c r="AC9" s="12"/>
+      <c r="X9" s="20"/>
+      <c r="Y9" s="12"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="12"/>
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="80"/>
     </row>
     <row r="10" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+      <c r="A10" s="7">
         <v>7</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="9">
         <v>1194</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="10">
         <v>1284</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="9">
         <v>1541</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="32">
         <v>6</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="11">
         <v>7</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="H10" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="I10" s="12">
+      <c r="I10" s="9">
         <v>60</v>
       </c>
-      <c r="J10" s="17">
+      <c r="J10" s="13">
         <v>65</v>
       </c>
-      <c r="K10" s="12">
+      <c r="K10" s="9">
         <v>66</v>
       </c>
-      <c r="L10" s="18">
+      <c r="L10" s="14">
         <v>0.5</v>
       </c>
-      <c r="M10" s="48">
+      <c r="M10" s="41">
         <f t="shared" si="0"/>
         <v>144230.76923076925</v>
       </c>
-      <c r="N10" s="19">
+      <c r="N10" s="15">
         <v>150000</v>
       </c>
-      <c r="O10" s="48">
+      <c r="O10" s="41">
         <f t="shared" si="1"/>
         <v>151153.84615384616</v>
       </c>
-      <c r="P10" s="20">
+      <c r="P10" s="16">
         <v>11</v>
       </c>
-      <c r="Q10" s="21">
+      <c r="Q10" s="17">
         <v>7</v>
       </c>
-      <c r="R10" s="22" t="s">
+      <c r="R10" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="S10" s="18">
+      <c r="S10" s="14">
         <v>19</v>
       </c>
-      <c r="T10" s="22">
+      <c r="T10" s="18">
         <v>21</v>
       </c>
-      <c r="U10" s="18">
+      <c r="U10" s="14">
         <v>25</v>
       </c>
-      <c r="V10" s="18">
+      <c r="V10" s="14">
         <v>11</v>
       </c>
-      <c r="W10" s="23">
+      <c r="W10" s="19">
         <v>0.2</v>
       </c>
-      <c r="X10" s="24"/>
-      <c r="Y10" s="16"/>
-      <c r="Z10" s="12"/>
-      <c r="AA10" s="16"/>
-      <c r="AB10" s="12"/>
-      <c r="AC10" s="12"/>
+      <c r="X10" s="20"/>
+      <c r="Y10" s="12"/>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="12"/>
+      <c r="AB10" s="9"/>
+      <c r="AC10" s="80"/>
     </row>
     <row r="11" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
+      <c r="A11" s="7">
         <v>8</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="9">
         <v>182</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="10">
         <v>200</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="9">
         <v>256</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11" s="32">
         <v>6</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="11">
         <v>8</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="H11" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="9">
         <v>26</v>
       </c>
-      <c r="J11" s="17">
+      <c r="J11" s="13">
         <v>26</v>
       </c>
-      <c r="K11" s="12">
+      <c r="K11" s="9">
         <v>26</v>
       </c>
-      <c r="L11" s="18">
+      <c r="L11" s="14">
         <v>0.5</v>
       </c>
-      <c r="M11" s="48">
+      <c r="M11" s="41">
         <f t="shared" si="0"/>
         <v>60000</v>
       </c>
-      <c r="N11" s="19">
+      <c r="N11" s="15">
         <v>60000</v>
       </c>
-      <c r="O11" s="48">
+      <c r="O11" s="41">
         <f t="shared" si="1"/>
         <v>60000</v>
       </c>
-      <c r="P11" s="20">
+      <c r="P11" s="16">
         <v>12</v>
       </c>
-      <c r="Q11" s="21">
+      <c r="Q11" s="17">
         <v>8</v>
       </c>
-      <c r="R11" s="22" t="s">
+      <c r="R11" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="S11" s="18">
+      <c r="S11" s="14">
         <v>20</v>
       </c>
-      <c r="T11" s="22">
+      <c r="T11" s="18">
         <v>21</v>
       </c>
-      <c r="U11" s="18">
+      <c r="U11" s="14">
         <v>22</v>
       </c>
-      <c r="V11" s="18">
+      <c r="V11" s="14">
         <v>12</v>
       </c>
-      <c r="W11" s="23">
+      <c r="W11" s="19">
         <v>0.25</v>
       </c>
-      <c r="X11" s="24"/>
-      <c r="Y11" s="16"/>
-      <c r="Z11" s="12"/>
-      <c r="AA11" s="16"/>
-      <c r="AB11" s="12"/>
-      <c r="AC11" s="12"/>
+      <c r="X11" s="20"/>
+      <c r="Y11" s="12"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="12"/>
+      <c r="AB11" s="9"/>
+      <c r="AC11" s="80"/>
     </row>
     <row r="12" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
+      <c r="A12" s="7">
         <v>9</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="9">
         <v>363</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="10">
         <v>395</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="9">
         <v>486</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="32">
         <v>6</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G12" s="11">
         <v>9</v>
       </c>
-      <c r="H12" s="16" t="s">
+      <c r="H12" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="9">
         <v>27</v>
       </c>
-      <c r="J12" s="17">
+      <c r="J12" s="13">
         <v>33</v>
       </c>
-      <c r="K12" s="12">
+      <c r="K12" s="9">
         <v>33</v>
       </c>
-      <c r="L12" s="18">
+      <c r="L12" s="14">
         <v>0.5</v>
       </c>
-      <c r="M12" s="48">
+      <c r="M12" s="41">
         <f t="shared" si="0"/>
         <v>90909.090909090912</v>
       </c>
-      <c r="N12" s="19">
+      <c r="N12" s="15">
         <v>100000</v>
       </c>
-      <c r="O12" s="48">
+      <c r="O12" s="41">
         <f t="shared" si="1"/>
         <v>100000</v>
       </c>
-      <c r="P12" s="20">
+      <c r="P12" s="16">
         <v>14</v>
       </c>
-      <c r="Q12" s="21">
+      <c r="Q12" s="17">
         <v>9</v>
       </c>
-      <c r="R12" s="22" t="s">
+      <c r="R12" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="S12" s="18">
+      <c r="S12" s="14">
         <v>20</v>
       </c>
-      <c r="T12" s="22">
+      <c r="T12" s="18">
         <v>21</v>
       </c>
-      <c r="U12" s="18">
+      <c r="U12" s="14">
         <v>23</v>
       </c>
-      <c r="V12" s="18">
+      <c r="V12" s="14">
         <v>14</v>
       </c>
-      <c r="W12" s="23">
+      <c r="W12" s="19">
         <v>0.05</v>
       </c>
-      <c r="X12" s="24"/>
-      <c r="Y12" s="16"/>
-      <c r="Z12" s="12"/>
-      <c r="AA12" s="16"/>
-      <c r="AB12" s="12"/>
-      <c r="AC12" s="12"/>
+      <c r="X12" s="20"/>
+      <c r="Y12" s="12"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="12"/>
+      <c r="AB12" s="9"/>
+      <c r="AC12" s="80"/>
     </row>
     <row r="13" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
+      <c r="A13" s="7">
         <v>10</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="9">
         <v>234</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="10">
         <v>260</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="9">
         <v>325</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13" s="32">
         <v>6</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="11">
         <v>10</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="9">
         <v>23</v>
       </c>
-      <c r="J13" s="17">
+      <c r="J13" s="13">
         <v>26</v>
       </c>
-      <c r="K13" s="12">
+      <c r="K13" s="9">
         <v>27</v>
       </c>
-      <c r="L13" s="18">
+      <c r="L13" s="14">
         <v>0.5</v>
       </c>
-      <c r="M13" s="48">
+      <c r="M13" s="41">
         <f t="shared" si="0"/>
         <v>235576.92307692306</v>
       </c>
-      <c r="N13" s="19">
+      <c r="N13" s="15">
         <v>250000</v>
       </c>
-      <c r="O13" s="48">
+      <c r="O13" s="41">
         <f t="shared" si="1"/>
         <v>254807.69230769228</v>
       </c>
-      <c r="P13" s="20">
+      <c r="P13" s="16">
         <v>15</v>
       </c>
-      <c r="Q13" s="21">
+      <c r="Q13" s="17">
         <v>10</v>
       </c>
-      <c r="R13" s="22" t="s">
+      <c r="R13" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="S13" s="18">
+      <c r="S13" s="14">
         <v>13</v>
       </c>
-      <c r="T13" s="22">
+      <c r="T13" s="18">
         <v>14</v>
       </c>
-      <c r="U13" s="18">
+      <c r="U13" s="14">
         <v>15</v>
       </c>
-      <c r="V13" s="18">
+      <c r="V13" s="14">
         <v>15</v>
       </c>
-      <c r="W13" s="23">
+      <c r="W13" s="19">
         <v>0.05</v>
       </c>
-      <c r="X13" s="24"/>
-      <c r="Y13" s="16"/>
-      <c r="Z13" s="12"/>
-      <c r="AA13" s="16"/>
-      <c r="AB13" s="12"/>
-      <c r="AC13" s="12"/>
+      <c r="X13" s="20"/>
+      <c r="Y13" s="12"/>
+      <c r="Z13" s="9"/>
+      <c r="AA13" s="12"/>
+      <c r="AB13" s="9"/>
+      <c r="AC13" s="80"/>
     </row>
     <row r="14" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
+      <c r="A14" s="7">
         <v>11</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="9">
         <v>305</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="10">
         <v>335</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="9">
         <v>425</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="32">
         <v>6</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14" s="11">
         <v>11</v>
       </c>
-      <c r="H14" s="16" t="s">
+      <c r="H14" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="9">
         <v>103</v>
       </c>
-      <c r="J14" s="17">
+      <c r="J14" s="13">
         <v>104</v>
       </c>
-      <c r="K14" s="12">
+      <c r="K14" s="9">
         <v>114</v>
       </c>
-      <c r="L14" s="18">
+      <c r="L14" s="14">
         <v>0.5</v>
       </c>
-      <c r="M14" s="48">
+      <c r="M14" s="41">
         <f t="shared" si="0"/>
         <v>199038.46153846153</v>
       </c>
-      <c r="N14" s="19">
+      <c r="N14" s="15">
         <v>200000</v>
       </c>
-      <c r="O14" s="48">
+      <c r="O14" s="41">
         <f t="shared" si="1"/>
         <v>209615.38461538462</v>
       </c>
-      <c r="P14" s="20">
+      <c r="P14" s="16">
         <v>16</v>
       </c>
-      <c r="Q14" s="21">
+      <c r="Q14" s="17">
         <v>11</v>
       </c>
-      <c r="R14" s="22" t="s">
+      <c r="R14" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="S14" s="18">
+      <c r="S14" s="14">
         <v>33</v>
       </c>
-      <c r="T14" s="22">
+      <c r="T14" s="18">
         <v>35</v>
       </c>
-      <c r="U14" s="18">
+      <c r="U14" s="14">
         <v>41</v>
       </c>
-      <c r="V14" s="18">
+      <c r="V14" s="14">
         <v>16</v>
       </c>
-      <c r="W14" s="23">
+      <c r="W14" s="19">
         <v>0.1</v>
       </c>
-      <c r="X14" s="24"/>
-      <c r="Y14" s="16"/>
-      <c r="Z14" s="12"/>
-      <c r="AA14" s="16"/>
-      <c r="AB14" s="12"/>
-      <c r="AC14" s="12"/>
+      <c r="X14" s="20"/>
+      <c r="Y14" s="12"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="12"/>
+      <c r="AB14" s="9"/>
+      <c r="AC14" s="80"/>
     </row>
     <row r="15" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
+      <c r="A15" s="7">
         <v>12</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="9">
         <v>120</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="10">
         <v>128</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="9">
         <v>155</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="F15" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G15" s="11">
         <v>12</v>
       </c>
-      <c r="H15" s="16" t="s">
+      <c r="H15" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="9">
         <v>7</v>
       </c>
-      <c r="J15" s="17">
+      <c r="J15" s="13">
         <v>7</v>
       </c>
-      <c r="K15" s="12">
+      <c r="K15" s="9">
         <v>7</v>
       </c>
-      <c r="L15" s="18">
+      <c r="L15" s="14">
         <v>0.5</v>
       </c>
-      <c r="M15" s="48">
+      <c r="M15" s="41">
         <f t="shared" si="0"/>
         <v>30000</v>
       </c>
-      <c r="N15" s="19">
+      <c r="N15" s="15">
         <v>30000</v>
       </c>
-      <c r="O15" s="48">
+      <c r="O15" s="41">
         <f t="shared" si="1"/>
         <v>30000</v>
       </c>
-      <c r="P15" s="20">
+      <c r="P15" s="16">
         <v>18</v>
       </c>
-      <c r="Q15" s="21">
+      <c r="Q15" s="17">
         <v>12</v>
       </c>
-      <c r="R15" s="22" t="s">
+      <c r="R15" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="S15" s="18">
+      <c r="S15" s="14">
         <v>20</v>
       </c>
-      <c r="T15" s="22">
+      <c r="T15" s="18">
         <v>21</v>
       </c>
-      <c r="U15" s="18">
+      <c r="U15" s="14">
         <v>21</v>
       </c>
-      <c r="V15" s="18">
+      <c r="V15" s="14">
         <v>18</v>
       </c>
-      <c r="W15" s="23">
+      <c r="W15" s="19">
         <v>0.25</v>
       </c>
-      <c r="X15" s="24"/>
-      <c r="Y15" s="16"/>
-      <c r="Z15" s="12"/>
-      <c r="AA15" s="16"/>
-      <c r="AB15" s="12"/>
-      <c r="AC15" s="12"/>
+      <c r="X15" s="20"/>
+      <c r="Y15" s="12"/>
+      <c r="Z15" s="9"/>
+      <c r="AA15" s="12"/>
+      <c r="AB15" s="9"/>
+      <c r="AC15" s="80"/>
     </row>
     <row r="16" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
+      <c r="A16" s="7">
         <v>13</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="9">
         <v>0</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="10">
         <v>0</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="9">
         <v>0</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="32">
         <v>12</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="11">
         <v>13</v>
       </c>
-      <c r="H16" s="16" t="s">
+      <c r="H16" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="I16" s="12">
+      <c r="I16" s="9">
         <v>49</v>
       </c>
-      <c r="J16" s="17">
+      <c r="J16" s="13">
         <v>52</v>
       </c>
-      <c r="K16" s="12">
+      <c r="K16" s="9">
         <v>52</v>
       </c>
-      <c r="L16" s="18">
+      <c r="L16" s="14">
         <v>0.5</v>
       </c>
-      <c r="M16" s="48">
+      <c r="M16" s="41">
         <f t="shared" si="0"/>
         <v>121394.23076923077</v>
       </c>
-      <c r="N16" s="19">
+      <c r="N16" s="15">
         <v>125000</v>
       </c>
-      <c r="O16" s="48">
+      <c r="O16" s="41">
         <f t="shared" si="1"/>
         <v>125000</v>
       </c>
-      <c r="P16" s="20">
+      <c r="P16" s="16">
         <v>20</v>
       </c>
-      <c r="Q16" s="21">
+      <c r="Q16" s="17">
         <v>13</v>
       </c>
-      <c r="R16" s="22" t="s">
+      <c r="R16" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="S16" s="18">
+      <c r="S16" s="14">
         <v>13</v>
       </c>
-      <c r="T16" s="22">
+      <c r="T16" s="18">
         <v>14</v>
       </c>
-      <c r="U16" s="18">
+      <c r="U16" s="14">
         <v>14</v>
       </c>
-      <c r="V16" s="18">
+      <c r="V16" s="14">
         <v>20</v>
       </c>
-      <c r="W16" s="23">
+      <c r="W16" s="19">
         <v>0.05</v>
       </c>
-      <c r="X16" s="24"/>
-      <c r="Y16" s="16"/>
-      <c r="Z16" s="12"/>
-      <c r="AA16" s="16"/>
-      <c r="AB16" s="12"/>
-      <c r="AC16" s="12"/>
+      <c r="X16" s="20"/>
+      <c r="Y16" s="12"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" s="12"/>
+      <c r="AB16" s="9"/>
+      <c r="AC16" s="80"/>
     </row>
     <row r="17" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
+      <c r="A17" s="7">
         <v>14</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="9">
         <v>241</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="10">
         <v>251</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="9">
         <v>279</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="32">
         <v>6</v>
       </c>
-      <c r="G17" s="15">
+      <c r="G17" s="11">
         <v>14</v>
       </c>
-      <c r="H17" s="16" t="s">
+      <c r="H17" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="9">
         <v>42</v>
       </c>
-      <c r="J17" s="17">
+      <c r="J17" s="13">
         <v>52</v>
       </c>
-      <c r="K17" s="12">
+      <c r="K17" s="9">
         <v>55</v>
       </c>
-      <c r="L17" s="18">
+      <c r="L17" s="14">
         <v>0.5</v>
       </c>
-      <c r="M17" s="48">
+      <c r="M17" s="41">
         <f t="shared" si="0"/>
         <v>67788.461538461546</v>
       </c>
-      <c r="N17" s="19">
+      <c r="N17" s="15">
         <v>75000</v>
       </c>
-      <c r="O17" s="48">
+      <c r="O17" s="41">
         <f t="shared" si="1"/>
         <v>77163.461538461532</v>
       </c>
-      <c r="P17" s="20">
+      <c r="P17" s="16">
         <v>21</v>
       </c>
-      <c r="Q17" s="21">
+      <c r="Q17" s="17">
         <v>14</v>
       </c>
-      <c r="R17" s="22" t="s">
+      <c r="R17" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="S17" s="18">
+      <c r="S17" s="14">
         <v>13</v>
       </c>
-      <c r="T17" s="22">
+      <c r="T17" s="18">
         <v>14</v>
       </c>
-      <c r="U17" s="18">
+      <c r="U17" s="14">
         <v>14</v>
       </c>
-      <c r="V17" s="18">
+      <c r="V17" s="14">
         <v>21</v>
       </c>
-      <c r="W17" s="23">
+      <c r="W17" s="19">
         <v>0.05</v>
       </c>
-      <c r="X17" s="24"/>
-      <c r="Y17" s="16"/>
-      <c r="Z17" s="12"/>
-      <c r="AA17" s="16"/>
-      <c r="AB17" s="12"/>
-      <c r="AC17" s="12"/>
+      <c r="X17" s="20"/>
+      <c r="Y17" s="12"/>
+      <c r="Z17" s="9"/>
+      <c r="AA17" s="12"/>
+      <c r="AB17" s="9"/>
+      <c r="AC17" s="80"/>
     </row>
     <row r="18" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
+      <c r="A18" s="7">
         <v>15</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="9">
         <v>209</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="10">
         <v>220</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="9">
         <v>279</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F18" s="36">
         <v>14</v>
       </c>
-      <c r="G18" s="15">
+      <c r="G18" s="11">
         <v>15</v>
       </c>
-      <c r="H18" s="16" t="s">
+      <c r="H18" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="I18" s="12">
+      <c r="I18" s="9">
         <v>36</v>
       </c>
-      <c r="J18" s="17">
+      <c r="J18" s="13">
         <v>39</v>
       </c>
-      <c r="K18" s="12">
+      <c r="K18" s="9">
         <v>43</v>
       </c>
-      <c r="L18" s="18">
+      <c r="L18" s="14">
         <v>0.5</v>
       </c>
-      <c r="M18" s="48">
+      <c r="M18" s="41">
         <f t="shared" si="0"/>
         <v>1442307.6923076923</v>
       </c>
-      <c r="N18" s="19">
+      <c r="N18" s="15">
         <v>1500000</v>
       </c>
-      <c r="O18" s="48">
+      <c r="O18" s="41">
         <f t="shared" si="1"/>
         <v>1576923.076923077</v>
       </c>
-      <c r="P18" s="20">
+      <c r="P18" s="16">
         <v>22</v>
       </c>
-      <c r="Q18" s="21">
+      <c r="Q18" s="17">
         <v>15</v>
       </c>
-      <c r="R18" s="22" t="s">
+      <c r="R18" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="S18" s="18">
+      <c r="S18" s="14">
         <v>65</v>
       </c>
-      <c r="T18" s="22">
+      <c r="T18" s="18">
         <v>70</v>
       </c>
-      <c r="U18" s="18">
+      <c r="U18" s="14">
         <v>71</v>
       </c>
-      <c r="V18" s="18">
+      <c r="V18" s="14">
         <v>22</v>
       </c>
-      <c r="W18" s="23">
+      <c r="W18" s="19">
         <v>0.02</v>
       </c>
-      <c r="X18" s="24"/>
-      <c r="Y18" s="16"/>
-      <c r="Z18" s="12"/>
-      <c r="AA18" s="16"/>
-      <c r="AB18" s="12"/>
-      <c r="AC18" s="12"/>
+      <c r="X18" s="20"/>
+      <c r="Y18" s="12"/>
+      <c r="Z18" s="9"/>
+      <c r="AA18" s="12"/>
+      <c r="AB18" s="9"/>
+      <c r="AC18" s="80"/>
     </row>
     <row r="19" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
+      <c r="A19" s="7">
         <v>16</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="9">
         <v>667</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="10">
         <v>674</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="9">
         <v>782</v>
       </c>
-      <c r="F19" s="25">
+      <c r="F19" s="32">
         <v>14</v>
       </c>
-      <c r="G19" s="15">
+      <c r="G19" s="11">
         <v>16</v>
       </c>
-      <c r="H19" s="16" t="s">
+      <c r="H19" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="I19" s="12">
+      <c r="I19" s="9">
         <v>31</v>
       </c>
-      <c r="J19" s="17">
+      <c r="J19" s="13">
         <v>39</v>
       </c>
-      <c r="K19" s="12">
+      <c r="K19" s="9">
         <v>42</v>
       </c>
-      <c r="L19" s="18">
+      <c r="L19" s="14">
         <v>0.5</v>
       </c>
-      <c r="M19" s="48">
+      <c r="M19" s="41">
         <f t="shared" si="0"/>
         <v>134615.38461538462</v>
       </c>
-      <c r="N19" s="19">
+      <c r="N19" s="15">
         <v>150000</v>
       </c>
-      <c r="O19" s="48">
+      <c r="O19" s="41">
         <f t="shared" si="1"/>
         <v>155769.23076923078</v>
       </c>
-      <c r="P19" s="20">
+      <c r="P19" s="16">
         <v>23</v>
       </c>
-      <c r="Q19" s="21">
+      <c r="Q19" s="17">
         <v>16</v>
       </c>
-      <c r="R19" s="22" t="s">
+      <c r="R19" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="S19" s="18">
+      <c r="S19" s="14">
         <v>25</v>
       </c>
-      <c r="T19" s="22">
+      <c r="T19" s="18">
         <v>28</v>
       </c>
-      <c r="U19" s="18">
+      <c r="U19" s="14">
         <v>32</v>
       </c>
-      <c r="V19" s="18">
+      <c r="V19" s="14">
         <v>23</v>
       </c>
-      <c r="W19" s="23">
+      <c r="W19" s="19">
         <v>0.05</v>
       </c>
-      <c r="X19" s="24"/>
-      <c r="Y19" s="16"/>
-      <c r="Z19" s="12"/>
-      <c r="AA19" s="16"/>
-      <c r="AB19" s="12"/>
-      <c r="AC19" s="12"/>
+      <c r="X19" s="20"/>
+      <c r="Y19" s="12"/>
+      <c r="Z19" s="9"/>
+      <c r="AA19" s="12"/>
+      <c r="AB19" s="9"/>
+      <c r="AC19" s="80"/>
     </row>
     <row r="20" spans="1:29" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
+      <c r="A20" s="7">
         <v>17</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="9">
         <v>0</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20" s="10">
         <v>0</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E20" s="9">
         <v>0</v>
       </c>
-      <c r="F20" s="25">
+      <c r="F20" s="32">
         <v>16</v>
       </c>
-      <c r="G20" s="15">
+      <c r="G20" s="11">
         <v>17</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="H20" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="I20" s="12">
+      <c r="I20" s="9">
         <v>52</v>
       </c>
-      <c r="J20" s="17">
+      <c r="J20" s="13">
         <v>52</v>
       </c>
-      <c r="K20" s="12">
+      <c r="K20" s="9">
         <v>55</v>
       </c>
-      <c r="L20" s="18">
+      <c r="L20" s="14">
         <v>0.5</v>
       </c>
-      <c r="M20" s="48">
+      <c r="M20" s="41">
         <f t="shared" si="0"/>
         <v>200000</v>
       </c>
-      <c r="N20" s="19">
+      <c r="N20" s="15">
         <v>200000</v>
       </c>
-      <c r="O20" s="48">
+      <c r="O20" s="41">
         <f t="shared" si="1"/>
         <v>205769.23076923075</v>
       </c>
-      <c r="P20" s="20">
+      <c r="P20" s="16">
         <v>26</v>
       </c>
-      <c r="Q20" s="21">
+      <c r="Q20" s="17">
         <v>17</v>
       </c>
-      <c r="R20" s="22" t="s">
+      <c r="R20" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="S20" s="18">
+      <c r="S20" s="14">
         <v>39</v>
       </c>
-      <c r="T20" s="22">
+      <c r="T20" s="18">
         <v>42</v>
       </c>
-      <c r="U20" s="18">
+      <c r="U20" s="14">
         <v>47</v>
       </c>
-      <c r="V20" s="18">
+      <c r="V20" s="14">
         <v>26</v>
       </c>
-      <c r="W20" s="23">
+      <c r="W20" s="19">
         <v>0.02</v>
       </c>
-      <c r="X20" s="24"/>
-      <c r="Y20" s="16"/>
-      <c r="Z20" s="12"/>
-      <c r="AA20" s="16"/>
-      <c r="AB20" s="12"/>
-      <c r="AC20" s="12"/>
+      <c r="X20" s="20"/>
+      <c r="Y20" s="12"/>
+      <c r="Z20" s="9"/>
+      <c r="AA20" s="12"/>
+      <c r="AB20" s="9"/>
+      <c r="AC20" s="80"/>
     </row>
     <row r="21" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
+      <c r="A21" s="7">
         <v>18</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="9">
         <v>120</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="10">
         <v>130</v>
       </c>
-      <c r="E21" s="12">
+      <c r="E21" s="9">
         <v>147</v>
       </c>
-      <c r="F21" s="25">
+      <c r="F21" s="32">
         <v>17</v>
       </c>
-      <c r="G21" s="15">
+      <c r="G21" s="11">
         <v>18</v>
       </c>
-      <c r="H21" s="16" t="s">
+      <c r="H21" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="I21" s="12">
+      <c r="I21" s="9">
         <v>22</v>
       </c>
-      <c r="J21" s="17">
+      <c r="J21" s="13">
         <v>26</v>
       </c>
-      <c r="K21" s="12">
+      <c r="K21" s="9">
         <v>27</v>
       </c>
-      <c r="L21" s="18">
+      <c r="L21" s="14">
         <v>0.5</v>
       </c>
-      <c r="M21" s="48">
+      <c r="M21" s="41">
         <f t="shared" si="0"/>
         <v>69230.769230769234</v>
       </c>
-      <c r="N21" s="19">
+      <c r="N21" s="15">
         <v>75000</v>
       </c>
-      <c r="O21" s="48">
+      <c r="O21" s="41">
         <f t="shared" si="1"/>
         <v>76442.307692307688</v>
       </c>
-      <c r="P21" s="20">
+      <c r="P21" s="16">
         <v>28</v>
       </c>
-      <c r="Q21" s="21">
+      <c r="Q21" s="17">
         <v>18</v>
       </c>
-      <c r="R21" s="22" t="s">
+      <c r="R21" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="S21" s="18">
+      <c r="S21" s="14">
         <v>13</v>
       </c>
-      <c r="T21" s="22">
+      <c r="T21" s="18">
         <v>14</v>
       </c>
-      <c r="U21" s="18">
+      <c r="U21" s="14">
         <v>17</v>
       </c>
-      <c r="V21" s="18">
+      <c r="V21" s="14">
         <v>28</v>
       </c>
-      <c r="W21" s="23">
+      <c r="W21" s="19">
         <v>0.05</v>
       </c>
-      <c r="X21" s="24"/>
-      <c r="Y21" s="16"/>
-      <c r="Z21" s="12"/>
-      <c r="AA21" s="16"/>
-      <c r="AB21" s="12"/>
-      <c r="AC21" s="12"/>
+      <c r="X21" s="20"/>
+      <c r="Y21" s="12"/>
+      <c r="Z21" s="9"/>
+      <c r="AA21" s="12"/>
+      <c r="AB21" s="9"/>
+      <c r="AC21" s="80"/>
     </row>
     <row r="22" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="10">
+      <c r="A22" s="7">
         <v>19</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="9">
         <v>0</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="10">
         <v>0</v>
       </c>
-      <c r="E22" s="12">
+      <c r="E22" s="9">
         <v>0</v>
       </c>
-      <c r="F22" s="25">
+      <c r="F22" s="32">
         <v>18</v>
       </c>
-      <c r="G22" s="28">
+      <c r="G22" s="22">
         <v>19</v>
       </c>
-      <c r="H22" s="29" t="s">
+      <c r="H22" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="I22" s="30">
+      <c r="I22" s="24">
         <v>5</v>
       </c>
-      <c r="J22" s="31">
+      <c r="J22" s="25">
         <v>7</v>
       </c>
-      <c r="K22" s="30">
+      <c r="K22" s="24">
         <v>8</v>
       </c>
-      <c r="L22" s="32">
+      <c r="L22" s="26">
         <v>0.5</v>
       </c>
-      <c r="M22" s="48">
+      <c r="M22" s="41">
         <f t="shared" si="0"/>
         <v>214285.71428571429</v>
       </c>
-      <c r="N22" s="32">
+      <c r="N22" s="26">
         <v>250000</v>
       </c>
-      <c r="O22" s="48">
+      <c r="O22" s="41">
         <f t="shared" si="1"/>
         <v>267857.14285714284</v>
       </c>
-      <c r="P22" s="33">
+      <c r="P22" s="27">
         <v>30</v>
       </c>
-      <c r="Q22" s="34">
+      <c r="Q22" s="28">
         <v>19</v>
       </c>
-      <c r="R22" s="35" t="s">
+      <c r="R22" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="S22" s="32">
+      <c r="S22" s="26">
         <v>130</v>
       </c>
-      <c r="T22" s="35">
+      <c r="T22" s="29">
         <v>140</v>
       </c>
-      <c r="U22" s="32">
+      <c r="U22" s="26">
         <v>160</v>
       </c>
-      <c r="V22" s="32">
+      <c r="V22" s="26">
         <v>30</v>
       </c>
-      <c r="W22" s="36">
+      <c r="W22" s="30">
         <v>0.01</v>
       </c>
-      <c r="X22" s="37"/>
-      <c r="Y22" s="29"/>
-      <c r="Z22" s="30"/>
-      <c r="AA22" s="16"/>
-      <c r="AB22" s="30"/>
-      <c r="AC22" s="30"/>
+      <c r="X22" s="31"/>
+      <c r="Y22" s="23"/>
+      <c r="Z22" s="24"/>
+      <c r="AA22" s="23"/>
+      <c r="AB22" s="24"/>
+      <c r="AC22" s="81"/>
     </row>
     <row r="23" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="10">
+      <c r="A23" s="7">
         <v>20</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="9">
         <v>519</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="10">
         <v>530</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="9">
         <v>620</v>
       </c>
-      <c r="F23" s="38">
+      <c r="F23" s="32">
         <v>13</v>
       </c>
-      <c r="G23" s="39"/>
-      <c r="L23" s="40"/>
-      <c r="M23" s="49"/>
-      <c r="N23" s="19"/>
-      <c r="O23" s="49"/>
-      <c r="P23" s="40"/>
-      <c r="Q23" s="40"/>
-      <c r="R23" s="40"/>
-      <c r="S23" s="40"/>
-      <c r="T23" s="40"/>
-      <c r="U23" s="40"/>
-      <c r="V23" s="40"/>
-      <c r="W23" s="40"/>
+      <c r="G23" s="33"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="42"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="42"/>
+      <c r="P23" s="34"/>
+      <c r="Q23" s="34"/>
+      <c r="R23" s="34"/>
+      <c r="S23" s="34"/>
+      <c r="T23" s="34"/>
+      <c r="U23" s="34"/>
+      <c r="V23" s="34"/>
+      <c r="W23" s="34"/>
     </row>
     <row r="24" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
+      <c r="A24" s="7">
         <v>21</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="9">
         <v>396</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D24" s="10">
         <v>400</v>
       </c>
-      <c r="E24" s="12">
+      <c r="E24" s="9">
         <v>460</v>
       </c>
-      <c r="F24" s="38">
+      <c r="F24" s="32">
         <v>6</v>
       </c>
-      <c r="G24" s="39"/>
-      <c r="L24" s="40"/>
-      <c r="M24" s="49"/>
-      <c r="N24" s="19"/>
-      <c r="O24" s="49"/>
-      <c r="P24" s="40"/>
-      <c r="Q24" s="40"/>
-      <c r="R24" s="40"/>
-      <c r="S24" s="40"/>
-      <c r="T24" s="40"/>
-      <c r="U24" s="40"/>
-      <c r="V24" s="40"/>
-      <c r="W24" s="40"/>
+      <c r="G24" s="33"/>
+      <c r="L24" s="34"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="34"/>
+      <c r="Q24" s="34"/>
+      <c r="R24" s="34"/>
+      <c r="S24" s="34"/>
+      <c r="T24" s="34"/>
+      <c r="U24" s="34"/>
+      <c r="V24" s="34"/>
+      <c r="W24" s="34"/>
     </row>
     <row r="25" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="10">
+      <c r="A25" s="7">
         <v>22</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="9">
         <v>326</v>
       </c>
-      <c r="D25" s="13">
+      <c r="D25" s="10">
         <v>340</v>
       </c>
-      <c r="E25" s="12">
+      <c r="E25" s="9">
         <v>415</v>
       </c>
-      <c r="F25" s="38">
+      <c r="F25" s="32">
         <v>6</v>
       </c>
-      <c r="G25" s="39"/>
-      <c r="L25" s="40"/>
-      <c r="M25" s="49"/>
-      <c r="O25" s="49"/>
-      <c r="P25" s="40"/>
-      <c r="Q25" s="40"/>
-      <c r="R25" s="40"/>
-      <c r="S25" s="40"/>
-      <c r="T25" s="40"/>
-      <c r="U25" s="40"/>
-      <c r="V25" s="40"/>
-      <c r="W25" s="40"/>
+      <c r="G25" s="33"/>
+      <c r="L25" s="34"/>
+      <c r="M25" s="42"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="34"/>
+      <c r="Q25" s="34"/>
+      <c r="R25" s="34"/>
+      <c r="S25" s="34"/>
+      <c r="T25" s="34"/>
+      <c r="U25" s="34"/>
+      <c r="V25" s="34"/>
+      <c r="W25" s="34"/>
     </row>
     <row r="26" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="10">
+      <c r="A26" s="7">
         <v>23</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="9">
         <v>856</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26" s="10">
         <v>930</v>
       </c>
-      <c r="E26" s="12">
+      <c r="E26" s="9">
         <v>1209</v>
       </c>
-      <c r="F26" s="38">
+      <c r="F26" s="32">
         <v>6</v>
       </c>
-      <c r="G26" s="39"/>
-      <c r="L26" s="40"/>
-      <c r="M26" s="49"/>
-      <c r="O26" s="49"/>
-      <c r="P26" s="40"/>
-      <c r="Q26" s="40"/>
-      <c r="R26" s="40"/>
-      <c r="S26" s="40"/>
-      <c r="T26" s="40"/>
-      <c r="U26" s="40"/>
-      <c r="V26" s="40"/>
-      <c r="W26" s="40"/>
+      <c r="G26" s="33"/>
+      <c r="L26" s="34"/>
+      <c r="M26" s="42"/>
+      <c r="O26" s="42"/>
+      <c r="P26" s="34"/>
+      <c r="Q26" s="34"/>
+      <c r="R26" s="34"/>
+      <c r="S26" s="34"/>
+      <c r="T26" s="34"/>
+      <c r="U26" s="34"/>
+      <c r="V26" s="34"/>
+      <c r="W26" s="34"/>
     </row>
     <row r="27" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="10">
+      <c r="A27" s="7">
         <v>24</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="12">
+      <c r="C27" s="9">
         <v>100</v>
       </c>
-      <c r="D27" s="13">
+      <c r="D27" s="10">
         <v>100</v>
       </c>
-      <c r="E27" s="12">
+      <c r="E27" s="9">
         <v>116</v>
       </c>
-      <c r="F27" s="38" t="s">
+      <c r="F27" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="G27" s="39"/>
-      <c r="L27" s="40"/>
-      <c r="M27" s="49"/>
-      <c r="O27" s="49"/>
-      <c r="P27" s="40"/>
-      <c r="Q27" s="40"/>
-      <c r="R27" s="40"/>
-      <c r="S27" s="40"/>
-      <c r="T27" s="40"/>
-      <c r="U27" s="40"/>
-      <c r="V27" s="40"/>
-      <c r="W27" s="40"/>
+      <c r="G27" s="33"/>
+      <c r="L27" s="34"/>
+      <c r="M27" s="42"/>
+      <c r="O27" s="42"/>
+      <c r="P27" s="34"/>
+      <c r="Q27" s="34"/>
+      <c r="R27" s="34"/>
+      <c r="S27" s="34"/>
+      <c r="T27" s="34"/>
+      <c r="U27" s="34"/>
+      <c r="V27" s="34"/>
+      <c r="W27" s="34"/>
     </row>
     <row r="28" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="10">
+      <c r="A28" s="7">
         <v>25</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="12">
+      <c r="C28" s="9">
         <v>0</v>
       </c>
-      <c r="D28" s="13">
+      <c r="D28" s="10">
         <v>0</v>
       </c>
-      <c r="E28" s="12">
+      <c r="E28" s="9">
         <v>0</v>
       </c>
-      <c r="F28" s="38">
+      <c r="F28" s="32">
         <v>24</v>
       </c>
-      <c r="G28" s="39"/>
-      <c r="L28" s="40"/>
-      <c r="M28" s="49"/>
-      <c r="O28" s="49"/>
-      <c r="P28" s="40"/>
-      <c r="Q28" s="40"/>
-      <c r="R28" s="40"/>
-      <c r="S28" s="40"/>
-      <c r="T28" s="40"/>
-      <c r="U28" s="40"/>
-      <c r="V28" s="40"/>
-      <c r="W28" s="40"/>
+      <c r="G28" s="33"/>
+      <c r="L28" s="34"/>
+      <c r="M28" s="42"/>
+      <c r="O28" s="42"/>
+      <c r="P28" s="34"/>
+      <c r="Q28" s="34"/>
+      <c r="R28" s="34"/>
+      <c r="S28" s="34"/>
+      <c r="T28" s="34"/>
+      <c r="U28" s="34"/>
+      <c r="V28" s="34"/>
+      <c r="W28" s="34"/>
     </row>
     <row r="29" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="10">
+      <c r="A29" s="7">
         <v>26</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="12">
+      <c r="C29" s="9">
         <v>380</v>
       </c>
-      <c r="D29" s="13">
+      <c r="D29" s="10">
         <v>400</v>
       </c>
-      <c r="E29" s="12">
+      <c r="E29" s="9">
         <v>508</v>
       </c>
-      <c r="F29" s="38">
+      <c r="F29" s="32">
         <v>25</v>
       </c>
-      <c r="G29" s="39"/>
-      <c r="L29" s="40"/>
-      <c r="M29" s="49"/>
-      <c r="O29" s="49"/>
-      <c r="P29" s="40"/>
-      <c r="Q29" s="40"/>
-      <c r="R29" s="40"/>
-      <c r="S29" s="40"/>
-      <c r="T29" s="40"/>
-      <c r="U29" s="40"/>
-      <c r="V29" s="40"/>
-      <c r="W29" s="40"/>
+      <c r="G29" s="33"/>
+      <c r="L29" s="34"/>
+      <c r="M29" s="42"/>
+      <c r="O29" s="42"/>
+      <c r="P29" s="34"/>
+      <c r="Q29" s="34"/>
+      <c r="R29" s="34"/>
+      <c r="S29" s="34"/>
+      <c r="T29" s="34"/>
+      <c r="U29" s="34"/>
+      <c r="V29" s="34"/>
+      <c r="W29" s="34"/>
     </row>
     <row r="30" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="10">
+      <c r="A30" s="7">
         <v>27</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="12">
+      <c r="C30" s="9">
         <v>0</v>
       </c>
-      <c r="D30" s="13">
+      <c r="D30" s="10">
         <v>0</v>
       </c>
-      <c r="E30" s="12">
+      <c r="E30" s="9">
         <v>0</v>
       </c>
-      <c r="F30" s="38" t="s">
+      <c r="F30" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="G30" s="39"/>
-      <c r="L30" s="40"/>
-      <c r="M30" s="49"/>
-      <c r="O30" s="49"/>
-      <c r="P30" s="40"/>
-      <c r="Q30" s="40"/>
-      <c r="R30" s="40"/>
-      <c r="S30" s="40"/>
-      <c r="T30" s="40"/>
-      <c r="U30" s="40"/>
-      <c r="V30" s="40"/>
-      <c r="W30" s="40"/>
+      <c r="G30" s="33"/>
+      <c r="L30" s="34"/>
+      <c r="M30" s="42"/>
+      <c r="O30" s="42"/>
+      <c r="P30" s="34"/>
+      <c r="Q30" s="34"/>
+      <c r="R30" s="34"/>
+      <c r="S30" s="34"/>
+      <c r="T30" s="34"/>
+      <c r="U30" s="34"/>
+      <c r="V30" s="34"/>
+      <c r="W30" s="34"/>
     </row>
     <row r="31" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="10">
+      <c r="A31" s="7">
         <v>28</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="12">
+      <c r="C31" s="9">
         <v>90</v>
       </c>
-      <c r="D31" s="13">
+      <c r="D31" s="10">
         <v>90</v>
       </c>
-      <c r="E31" s="12">
+      <c r="E31" s="9">
         <v>106</v>
       </c>
-      <c r="F31" s="38" t="s">
+      <c r="F31" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="G31" s="39"/>
-      <c r="L31" s="40"/>
-      <c r="M31" s="49"/>
-      <c r="O31" s="49"/>
-      <c r="P31" s="40"/>
-      <c r="Q31" s="40"/>
-      <c r="R31" s="40"/>
-      <c r="S31" s="40"/>
-      <c r="T31" s="40"/>
-      <c r="U31" s="40"/>
-      <c r="V31" s="40"/>
-      <c r="W31" s="40"/>
+      <c r="G31" s="33"/>
+      <c r="L31" s="34"/>
+      <c r="M31" s="42"/>
+      <c r="O31" s="42"/>
+      <c r="P31" s="34"/>
+      <c r="Q31" s="34"/>
+      <c r="R31" s="34"/>
+      <c r="S31" s="34"/>
+      <c r="T31" s="34"/>
+      <c r="U31" s="34"/>
+      <c r="V31" s="34"/>
+      <c r="W31" s="34"/>
     </row>
     <row r="32" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="10">
+      <c r="A32" s="7">
         <v>29</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="12">
+      <c r="C32" s="9">
         <v>0</v>
       </c>
-      <c r="D32" s="13">
+      <c r="D32" s="10">
         <v>0</v>
       </c>
-      <c r="E32" s="12">
+      <c r="E32" s="9">
         <v>0</v>
       </c>
-      <c r="F32" s="38">
+      <c r="F32" s="32">
         <v>28</v>
       </c>
-      <c r="G32" s="39"/>
-      <c r="L32" s="40"/>
-      <c r="M32" s="49"/>
-      <c r="O32" s="49"/>
-      <c r="P32" s="40"/>
-      <c r="Q32" s="40"/>
-      <c r="R32" s="40"/>
-      <c r="S32" s="40"/>
-      <c r="T32" s="40"/>
-      <c r="U32" s="40"/>
-      <c r="V32" s="40"/>
-      <c r="W32" s="40"/>
+      <c r="G32" s="33"/>
+      <c r="L32" s="34"/>
+      <c r="M32" s="42"/>
+      <c r="O32" s="42"/>
+      <c r="P32" s="34"/>
+      <c r="Q32" s="34"/>
+      <c r="R32" s="34"/>
+      <c r="S32" s="34"/>
+      <c r="T32" s="34"/>
+      <c r="U32" s="34"/>
+      <c r="V32" s="34"/>
+      <c r="W32" s="34"/>
     </row>
     <row r="33" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="10">
+      <c r="A33" s="7">
         <v>30</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="12">
+      <c r="C33" s="9">
         <v>19</v>
       </c>
-      <c r="D33" s="13">
+      <c r="D33" s="10">
         <v>20</v>
       </c>
-      <c r="E33" s="12">
+      <c r="E33" s="9">
         <v>23</v>
       </c>
-      <c r="F33" s="38">
+      <c r="F33" s="32">
         <v>29</v>
       </c>
-      <c r="G33" s="39"/>
-      <c r="L33" s="40"/>
-      <c r="M33" s="49"/>
-      <c r="O33" s="49"/>
-      <c r="P33" s="40"/>
-      <c r="Q33" s="40"/>
-      <c r="R33" s="40"/>
-      <c r="S33" s="40"/>
-      <c r="T33" s="40"/>
-      <c r="U33" s="40"/>
-      <c r="V33" s="40"/>
-      <c r="W33" s="40"/>
+      <c r="G33" s="33"/>
+      <c r="L33" s="34"/>
+      <c r="M33" s="42"/>
+      <c r="O33" s="42"/>
+      <c r="P33" s="34"/>
+      <c r="Q33" s="34"/>
+      <c r="R33" s="34"/>
+      <c r="S33" s="34"/>
+      <c r="T33" s="34"/>
+      <c r="U33" s="34"/>
+      <c r="V33" s="34"/>
+      <c r="W33" s="34"/>
     </row>
     <row r="34" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="10">
+      <c r="A34" s="7">
         <v>31</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="12">
+      <c r="C34" s="9">
         <v>57</v>
       </c>
-      <c r="D34" s="13">
+      <c r="D34" s="10">
         <v>61</v>
       </c>
-      <c r="E34" s="12">
+      <c r="E34" s="9">
         <v>71</v>
       </c>
-      <c r="F34" s="38">
+      <c r="F34" s="32">
         <v>30</v>
       </c>
-      <c r="G34" s="39"/>
-      <c r="L34" s="40"/>
-      <c r="M34" s="49"/>
-      <c r="O34" s="49"/>
-      <c r="P34" s="40"/>
-      <c r="Q34" s="40"/>
-      <c r="R34" s="40"/>
-      <c r="S34" s="40"/>
-      <c r="T34" s="40"/>
-      <c r="U34" s="40"/>
-      <c r="V34" s="40"/>
-      <c r="W34" s="40"/>
+      <c r="G34" s="33"/>
+      <c r="L34" s="34"/>
+      <c r="M34" s="42"/>
+      <c r="O34" s="42"/>
+      <c r="P34" s="34"/>
+      <c r="Q34" s="34"/>
+      <c r="R34" s="34"/>
+      <c r="S34" s="34"/>
+      <c r="T34" s="34"/>
+      <c r="U34" s="34"/>
+      <c r="V34" s="34"/>
+      <c r="W34" s="34"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A35" s="10">
+      <c r="A35" s="7">
         <v>32</v>
       </c>
-      <c r="B35" s="41" t="s">
+      <c r="B35" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="12">
+      <c r="C35" s="9">
         <v>29</v>
       </c>
-      <c r="D35" s="13">
+      <c r="D35" s="10">
         <v>30</v>
       </c>
-      <c r="E35" s="12">
+      <c r="E35" s="9">
         <v>35</v>
       </c>
-      <c r="F35" s="42">
+      <c r="F35" s="36">
         <v>31</v>
       </c>
-      <c r="G35" s="43"/>
-      <c r="L35" s="40"/>
-      <c r="M35" s="49"/>
-      <c r="O35" s="49"/>
-      <c r="P35" s="40"/>
-      <c r="Q35" s="40"/>
-      <c r="R35" s="40"/>
-      <c r="S35" s="40"/>
-      <c r="T35" s="40"/>
-      <c r="U35" s="40"/>
-      <c r="V35" s="40"/>
-      <c r="W35" s="40"/>
+      <c r="G35" s="37"/>
+      <c r="L35" s="34"/>
+      <c r="M35" s="42"/>
+      <c r="O35" s="42"/>
+      <c r="P35" s="34"/>
+      <c r="Q35" s="34"/>
+      <c r="R35" s="34"/>
+      <c r="S35" s="34"/>
+      <c r="T35" s="34"/>
+      <c r="U35" s="34"/>
+      <c r="V35" s="34"/>
+      <c r="W35" s="34"/>
     </row>
     <row r="36" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="10">
+      <c r="A36" s="7">
         <v>33</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="12">
+      <c r="C36" s="9">
         <v>82</v>
       </c>
-      <c r="D36" s="13">
+      <c r="D36" s="10">
         <v>90</v>
       </c>
-      <c r="E36" s="12">
+      <c r="E36" s="9">
         <v>107</v>
       </c>
-      <c r="F36" s="38">
+      <c r="F36" s="32">
         <v>31</v>
       </c>
-      <c r="G36" s="39"/>
-      <c r="L36" s="40"/>
-      <c r="M36" s="49"/>
-      <c r="O36" s="49"/>
-      <c r="P36" s="40"/>
-      <c r="Q36" s="40"/>
-      <c r="R36" s="40"/>
-      <c r="S36" s="40"/>
-      <c r="T36" s="40"/>
-      <c r="U36" s="40"/>
-      <c r="V36" s="40"/>
-      <c r="W36" s="40"/>
+      <c r="G36" s="33"/>
+      <c r="L36" s="34"/>
+      <c r="M36" s="42"/>
+      <c r="O36" s="42"/>
+      <c r="P36" s="34"/>
+      <c r="Q36" s="34"/>
+      <c r="R36" s="34"/>
+      <c r="S36" s="34"/>
+      <c r="T36" s="34"/>
+      <c r="U36" s="34"/>
+      <c r="V36" s="34"/>
+      <c r="W36" s="34"/>
     </row>
     <row r="37" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="10">
+      <c r="A37" s="7">
         <v>34</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="12">
+      <c r="C37" s="9">
         <v>119</v>
       </c>
-      <c r="D37" s="13">
+      <c r="D37" s="10">
         <v>120</v>
       </c>
-      <c r="E37" s="12">
+      <c r="E37" s="9">
         <v>149</v>
       </c>
-      <c r="F37" s="38">
+      <c r="F37" s="32">
         <v>30</v>
       </c>
-      <c r="G37" s="39"/>
-      <c r="L37" s="40"/>
-      <c r="M37" s="49"/>
-      <c r="O37" s="49"/>
-      <c r="P37" s="40"/>
-      <c r="Q37" s="40"/>
-      <c r="R37" s="40"/>
-      <c r="S37" s="40"/>
-      <c r="T37" s="40"/>
-      <c r="U37" s="40"/>
-      <c r="V37" s="40"/>
-      <c r="W37" s="40"/>
+      <c r="G37" s="33"/>
+      <c r="L37" s="34"/>
+      <c r="M37" s="42"/>
+      <c r="O37" s="42"/>
+      <c r="P37" s="34"/>
+      <c r="Q37" s="34"/>
+      <c r="R37" s="34"/>
+      <c r="S37" s="34"/>
+      <c r="T37" s="34"/>
+      <c r="U37" s="34"/>
+      <c r="V37" s="34"/>
+      <c r="W37" s="34"/>
     </row>
     <row r="38" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="10">
+      <c r="A38" s="7">
         <v>35</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="12">
+      <c r="C38" s="9">
         <v>0</v>
       </c>
-      <c r="D38" s="13">
+      <c r="D38" s="10">
         <v>0</v>
       </c>
-      <c r="E38" s="12">
+      <c r="E38" s="9">
         <v>0</v>
       </c>
-      <c r="F38" s="38">
+      <c r="F38" s="32">
         <v>33</v>
       </c>
-      <c r="G38" s="39"/>
-      <c r="L38" s="40"/>
-      <c r="M38" s="49"/>
-      <c r="O38" s="49"/>
-      <c r="P38" s="40"/>
-      <c r="Q38" s="40"/>
-      <c r="R38" s="40"/>
-      <c r="S38" s="40"/>
-      <c r="T38" s="40"/>
-      <c r="U38" s="40"/>
-      <c r="V38" s="40"/>
-      <c r="W38" s="40"/>
+      <c r="G38" s="33"/>
+      <c r="L38" s="34"/>
+      <c r="M38" s="42"/>
+      <c r="O38" s="42"/>
+      <c r="P38" s="34"/>
+      <c r="Q38" s="34"/>
+      <c r="R38" s="34"/>
+      <c r="S38" s="34"/>
+      <c r="T38" s="34"/>
+      <c r="U38" s="34"/>
+      <c r="V38" s="34"/>
+      <c r="W38" s="34"/>
     </row>
     <row r="39" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="10">
+      <c r="A39" s="7">
         <v>36</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="12">
+      <c r="C39" s="9">
         <v>18</v>
       </c>
-      <c r="D39" s="13">
+      <c r="D39" s="10">
         <v>20</v>
       </c>
-      <c r="E39" s="12">
+      <c r="E39" s="9">
         <v>24</v>
       </c>
-      <c r="F39" s="38">
+      <c r="F39" s="32">
         <v>35</v>
       </c>
-      <c r="G39" s="39"/>
-      <c r="L39" s="40"/>
-      <c r="M39" s="49"/>
-      <c r="O39" s="49"/>
-      <c r="P39" s="40"/>
-      <c r="Q39" s="40"/>
-      <c r="R39" s="40"/>
-      <c r="S39" s="40"/>
-      <c r="T39" s="40"/>
-      <c r="U39" s="40"/>
-      <c r="V39" s="40"/>
-      <c r="W39" s="40"/>
-    </row>
-    <row r="40" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="10">
+      <c r="G39" s="33"/>
+      <c r="L39" s="34"/>
+      <c r="M39" s="42"/>
+      <c r="O39" s="42"/>
+      <c r="P39" s="34"/>
+      <c r="Q39" s="34"/>
+      <c r="R39" s="34"/>
+      <c r="S39" s="34"/>
+      <c r="T39" s="34"/>
+      <c r="U39" s="34"/>
+      <c r="V39" s="34"/>
+      <c r="W39" s="34"/>
+    </row>
+    <row r="40" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="38">
         <v>37</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="12">
+      <c r="C40" s="24">
         <v>0</v>
       </c>
-      <c r="D40" s="13">
+      <c r="D40" s="40">
         <v>0</v>
       </c>
-      <c r="E40" s="12">
+      <c r="E40" s="24">
         <v>0</v>
       </c>
-      <c r="F40" s="38">
+      <c r="F40" s="77">
         <v>36</v>
       </c>
-      <c r="G40" s="39"/>
-      <c r="L40" s="40"/>
-      <c r="M40" s="49"/>
-      <c r="O40" s="49"/>
-      <c r="P40" s="40"/>
-      <c r="Q40" s="40"/>
-      <c r="R40" s="40"/>
-      <c r="S40" s="40"/>
-      <c r="T40" s="40"/>
-      <c r="U40" s="40"/>
-      <c r="V40" s="40"/>
-      <c r="W40" s="40"/>
-    </row>
-    <row r="41" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="44"/>
-      <c r="B41" s="45"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="46"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="47"/>
-      <c r="L41" s="40"/>
-      <c r="M41" s="49"/>
-      <c r="O41" s="49"/>
-      <c r="P41" s="40"/>
-      <c r="Q41" s="40"/>
-      <c r="R41" s="40"/>
-      <c r="S41" s="40"/>
-      <c r="T41" s="40"/>
-      <c r="U41" s="40"/>
-      <c r="V41" s="40"/>
-      <c r="W41" s="40"/>
+      <c r="G40" s="33"/>
+      <c r="L40" s="34"/>
+      <c r="M40" s="42"/>
+      <c r="O40" s="42"/>
+      <c r="P40" s="34"/>
+      <c r="Q40" s="34"/>
+      <c r="R40" s="34"/>
+      <c r="S40" s="34"/>
+      <c r="T40" s="34"/>
+      <c r="U40" s="34"/>
+      <c r="V40" s="34"/>
+      <c r="W40" s="34"/>
+    </row>
+    <row r="41" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="65"/>
+      <c r="B41" s="66"/>
+      <c r="C41" s="67"/>
+      <c r="D41" s="68"/>
+      <c r="E41" s="67"/>
+      <c r="F41" s="65"/>
+      <c r="L41" s="34"/>
+      <c r="M41" s="42"/>
+      <c r="O41" s="42"/>
+      <c r="P41" s="34"/>
+      <c r="Q41" s="34"/>
+      <c r="R41" s="34"/>
+      <c r="S41" s="34"/>
+      <c r="T41" s="34"/>
+      <c r="U41" s="34"/>
+      <c r="V41" s="34"/>
+      <c r="W41" s="34"/>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="L42" s="40"/>
-      <c r="M42" s="49"/>
-      <c r="O42" s="49"/>
-      <c r="P42" s="40"/>
-      <c r="Q42" s="40"/>
-      <c r="R42" s="40"/>
-      <c r="S42" s="40"/>
-      <c r="T42" s="40"/>
-      <c r="U42" s="40"/>
-      <c r="V42" s="40"/>
-      <c r="W42" s="40"/>
+      <c r="A42" s="65"/>
+      <c r="B42" s="65"/>
+      <c r="C42" s="65"/>
+      <c r="D42" s="65"/>
+      <c r="E42" s="65"/>
+      <c r="F42" s="65"/>
+      <c r="L42" s="34"/>
+      <c r="M42" s="42"/>
+      <c r="O42" s="42"/>
+      <c r="P42" s="34"/>
+      <c r="Q42" s="34"/>
+      <c r="R42" s="34"/>
+      <c r="S42" s="34"/>
+      <c r="T42" s="34"/>
+      <c r="U42" s="34"/>
+      <c r="V42" s="34"/>
+      <c r="W42" s="34"/>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="L43" s="40"/>
-      <c r="M43" s="49"/>
-      <c r="O43" s="49"/>
-      <c r="P43" s="40"/>
-      <c r="Q43" s="40"/>
-      <c r="R43" s="40"/>
-      <c r="S43" s="40"/>
-      <c r="T43" s="40"/>
-      <c r="U43" s="40"/>
-      <c r="V43" s="40"/>
-      <c r="W43" s="40"/>
+      <c r="L43" s="34"/>
+      <c r="M43" s="42"/>
+      <c r="O43" s="42"/>
+      <c r="P43" s="34"/>
+      <c r="Q43" s="34"/>
+      <c r="R43" s="34"/>
+      <c r="S43" s="34"/>
+      <c r="T43" s="34"/>
+      <c r="U43" s="34"/>
+      <c r="V43" s="34"/>
+      <c r="W43" s="34"/>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="L44" s="40"/>
-      <c r="M44" s="49"/>
-      <c r="O44" s="49"/>
-      <c r="P44" s="40"/>
-      <c r="Q44" s="40"/>
-      <c r="R44" s="40"/>
-      <c r="S44" s="40"/>
-      <c r="T44" s="40"/>
-      <c r="U44" s="40"/>
-      <c r="V44" s="40"/>
-      <c r="W44" s="40"/>
+      <c r="L44" s="34"/>
+      <c r="M44" s="42"/>
+      <c r="O44" s="42"/>
+      <c r="P44" s="34"/>
+      <c r="Q44" s="34"/>
+      <c r="R44" s="34"/>
+      <c r="S44" s="34"/>
+      <c r="T44" s="34"/>
+      <c r="U44" s="34"/>
+      <c r="V44" s="34"/>
+      <c r="W44" s="34"/>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="L45" s="40"/>
-      <c r="M45" s="49"/>
-      <c r="O45" s="49"/>
-      <c r="P45" s="40"/>
-      <c r="Q45" s="40"/>
-      <c r="R45" s="40"/>
-      <c r="S45" s="40"/>
-      <c r="T45" s="40"/>
-      <c r="U45" s="40"/>
-      <c r="V45" s="40"/>
-      <c r="W45" s="40"/>
+      <c r="L45" s="34"/>
+      <c r="M45" s="42"/>
+      <c r="O45" s="42"/>
+      <c r="P45" s="34"/>
+      <c r="Q45" s="34"/>
+      <c r="R45" s="34"/>
+      <c r="S45" s="34"/>
+      <c r="T45" s="34"/>
+      <c r="U45" s="34"/>
+      <c r="V45" s="34"/>
+      <c r="W45" s="34"/>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="L46" s="40"/>
-      <c r="M46" s="49"/>
-      <c r="O46" s="49"/>
-      <c r="P46" s="40"/>
-      <c r="Q46" s="40"/>
-      <c r="R46" s="40"/>
-      <c r="S46" s="40"/>
-      <c r="T46" s="40"/>
-      <c r="U46" s="40"/>
-      <c r="V46" s="40"/>
-      <c r="W46" s="40"/>
+      <c r="L46" s="34"/>
+      <c r="M46" s="42"/>
+      <c r="O46" s="42"/>
+      <c r="P46" s="34"/>
+      <c r="Q46" s="34"/>
+      <c r="R46" s="34"/>
+      <c r="S46" s="34"/>
+      <c r="T46" s="34"/>
+      <c r="U46" s="34"/>
+      <c r="V46" s="34"/>
+      <c r="W46" s="34"/>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="L47" s="40"/>
-      <c r="M47" s="49"/>
-      <c r="O47" s="49"/>
-      <c r="P47" s="40"/>
-      <c r="Q47" s="40"/>
-      <c r="R47" s="40"/>
-      <c r="S47" s="40"/>
-      <c r="T47" s="40"/>
-      <c r="U47" s="40"/>
-      <c r="V47" s="40"/>
-      <c r="W47" s="40"/>
+      <c r="L47" s="34"/>
+      <c r="M47" s="42"/>
+      <c r="O47" s="42"/>
+      <c r="P47" s="34"/>
+      <c r="Q47" s="34"/>
+      <c r="R47" s="34"/>
+      <c r="S47" s="34"/>
+      <c r="T47" s="34"/>
+      <c r="U47" s="34"/>
+      <c r="V47" s="34"/>
+      <c r="W47" s="34"/>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="L48" s="40"/>
-      <c r="M48" s="49"/>
-      <c r="O48" s="49"/>
-      <c r="P48" s="40"/>
-      <c r="Q48" s="40"/>
-      <c r="R48" s="40"/>
-      <c r="S48" s="40"/>
-      <c r="T48" s="40"/>
-      <c r="U48" s="40"/>
-      <c r="V48" s="40"/>
-      <c r="W48" s="40"/>
+      <c r="L48" s="34"/>
+      <c r="M48" s="42"/>
+      <c r="O48" s="42"/>
+      <c r="P48" s="34"/>
+      <c r="Q48" s="34"/>
+      <c r="R48" s="34"/>
+      <c r="S48" s="34"/>
+      <c r="T48" s="34"/>
+      <c r="U48" s="34"/>
+      <c r="V48" s="34"/>
+      <c r="W48" s="34"/>
     </row>
     <row r="49" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L49" s="40"/>
-      <c r="M49" s="49"/>
-      <c r="N49" s="40"/>
+      <c r="L49" s="34"/>
+      <c r="M49" s="42"/>
+      <c r="N49" s="34"/>
       <c r="O49" s="1"/>
     </row>
     <row r="50" spans="12:15" x14ac:dyDescent="0.25">
@@ -36602,17 +36678,11 @@
       <c r="O8281" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" insertColumns="0" insertRows="0"/>
+  <sheetProtection insertColumns="0" insertRows="0"/>
   <protectedRanges>
     <protectedRange sqref="J4:J22" name="Range1"/>
   </protectedRanges>
   <mergeCells count="18">
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="Y2:Y3"/>
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="AC2:AC3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="W2:W3"/>
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="L2:O2"/>
     <mergeCell ref="S2:U2"/>
@@ -36625,6 +36695,12 @@
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="W2:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated excel sheets with explanatory comments
</commit_message>
<xml_diff>
--- a/data/Case study 1.xlsx
+++ b/data/Case study 1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08AA6D8-4EC2-4316-9938-B1216461EE46}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62C5F6C-4F18-4583-A68E-A33FB265D29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,13 +27,344 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={5EBB22A6-E819-446D-8154-DE25FD7E6A82}</author>
+    <author>tc={77119148-1B5B-4125-8F01-307412D847BF}</author>
+    <author>tc={34228588-1163-43BB-A066-6E6CBEB9DE82}</author>
+    <author>tc={3166FD02-6A2F-4530-8FE7-452B92D57332}</author>
+    <author>tc={498AFDB6-4D70-414D-A23A-477BF3A55DD3}</author>
+    <author>tc={CAE32236-4976-460D-A21C-847ADD9F3F93}</author>
+    <author>tc={76097404-0119-4EF1-8361-CF42159A9F72}</author>
+    <author>tc={67C32F90-F393-4DFA-B39F-286253EDF727}</author>
+    <author>tc={A736116B-7089-4E7F-A0FC-748328F3EDED}</author>
+    <author>tc={B8899479-CE4F-40F6-A0C7-50DAC571D3C4}</author>
+    <author>tc={6CCA99F7-DA14-4459-8FD5-1B0864EF00F8}</author>
+    <author>tc={EF4EE362-5F89-4AF9-AC3E-CEB75088F726}</author>
+    <author>tc={CB203497-8043-4A3F-8BBF-A1A90A68AB14}</author>
+    <author>tc={B50C9B52-DF4C-4A39-8A57-0D501A9882F9}</author>
+    <author>tc={5301FCFF-164C-41C4-AC42-B19C77CCAFCF}</author>
+    <author>tc={44C21660-40A7-445E-8543-FF13C2067309}</author>
+    <author>tc={EFC09581-0698-442A-BCD5-86B53E94AD5B}</author>
+    <author>tc={9BD7A2D3-21C7-4A3A-AB77-E7076CBE9A54}</author>
+    <author>tc={9DA2A3F3-6BD2-494C-AF10-013A710097BC}</author>
+    <author>tc={4FE3E174-E4A9-423F-A48D-2D3CF7EF2390}</author>
+    <author>tc={0C024D35-B30C-499C-8366-794AE12585E6}</author>
+    <author>tc={9C5512D6-A380-4304-B147-51AFD5410007}</author>
+    <author>tc={32899173-A5AA-464F-8F9D-EEA5C1D31DBC}</author>
+    <author>tc={9A9F5103-A2D2-4EE0-BB31-DE11B9398886}</author>
+    <author>tc={36C57516-9BEA-4C79-B2AE-8F26F907B8EE}</author>
+    <author>tc={B2442A87-5162-43DD-AF9C-DF7C51A637C3}</author>
+    <author>tc={E74F529F-C920-4FFF-AC03-666348C1F3CA}</author>
+    <author>tc={4053F11A-ECEF-4B44-9FC5-4B64BAE74102}</author>
+    <author>tc={9E778C37-6EE2-4578-98D4-5BC7AB7B0BB6}</author>
+    <author>tc={D4E34699-714C-43AC-A14F-5B96DF915F7D}</author>
+    <author>tc={0A841E25-4AE6-4F68-979B-F02C85EF0E9C}</author>
+    <author>tc={34521897-0DFC-47DA-9314-BD8C94403FD4}</author>
+    <author>tc={7E35FC0E-6F9D-49A4-8589-5906257814F0}</author>
+    <author>tc={EA4240E9-7704-4713-8477-8A0FE2545DE9}</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{5EBB22A6-E819-446D-8154-DE25FD7E6A82}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    ID's of the activities. Keep the ID's in order starting from 1</t>
+      </text>
+    </comment>
+    <comment ref="B2" authorId="1" shapeId="0" xr:uid="{77119148-1B5B-4125-8F01-307412D847BF}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Description of project activities. It is not an essential input.</t>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="2" shapeId="0" xr:uid="{34228588-1163-43BB-A066-6E6CBEB9DE82}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Activities durations: three estimates
+Note that the three estimates must be in ascending order:
+minimum &lt;= Most-likely &lt;= maximum</t>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="3" shapeId="0" xr:uid="{3166FD02-6A2F-4530-8FE7-452B92D57332}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The ID's of the predecessor activities of each activity. This helps to define dependencies and to generate the project network diagram . This is a user input.
+You may insert more than one predecessor by separating them with a space or a comma</t>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="4" shapeId="0" xr:uid="{498AFDB6-4D70-414D-A23A-477BF3A55DD3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    ID's of the mitigation measures. Keep the ID's in order starting from 1</t>
+      </text>
+    </comment>
+    <comment ref="H2" authorId="5" shapeId="0" xr:uid="{CAE32236-4976-460D-A21C-847ADD9F3F93}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Description of mitigation measures activities. It is not an essential input.</t>
+      </text>
+    </comment>
+    <comment ref="I2" authorId="6" shapeId="0" xr:uid="{76097404-0119-4EF1-8361-CF42159A9F72}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Mitigation capacity of the mitigation measures: three estimates. 
+The mitigation capacity is the duration reduced from the total duration of the influenced activity
+Note that the three estimates must be in ascending order:
+minimum &lt;= Most-likely &lt;= maximum</t>
+      </text>
+    </comment>
+    <comment ref="L2" authorId="7" shapeId="0" xr:uid="{67C32F90-F393-4DFA-B39F-286253EDF727}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Cost of excecuting a mitigation measure</t>
+      </text>
+    </comment>
+    <comment ref="P2" authorId="8" shapeId="0" xr:uid="{A736116B-7089-4E7F-A0FC-748328F3EDED}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The ID's of activities that are influenced by each mitigation measure. 
+One Mitigation measure can influence (i.e., reduce the time of) one or more activities. You may insert more than one activity by separating them with a space or a comma.</t>
+      </text>
+    </comment>
+    <comment ref="Q2" authorId="9" shapeId="0" xr:uid="{B8899479-CE4F-40F6-A0C7-50DAC571D3C4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    ID's of the risk events. Keep the ID's in order starting from 1</t>
+      </text>
+    </comment>
+    <comment ref="R2" authorId="10" shapeId="0" xr:uid="{6CCA99F7-DA14-4459-8FD5-1B0864EF00F8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Description of risk events. It is not an essential input.</t>
+      </text>
+    </comment>
+    <comment ref="S2" authorId="11" shapeId="0" xr:uid="{EF4EE362-5F89-4AF9-AC3E-CEB75088F726}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The delay induced by each risk event: three estimates.
+Note that the three estimates must be in ascending order:
+minimum &lt;= Most-likely &lt;= maximum</t>
+      </text>
+    </comment>
+    <comment ref="V2" authorId="12" shapeId="0" xr:uid="{CB203497-8043-4A3F-8BBF-A1A90A68AB14}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The ID's of activities that are impacted by each risk event. 
+One risk event can impact (i.e., increase the time of) one or more activities. You may insert more than one activity by separating them with a space or a comma.</t>
+      </text>
+    </comment>
+    <comment ref="W2" authorId="13" shapeId="0" xr:uid="{B50C9B52-DF4C-4A39-8A57-0D501A9882F9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is the probability that a risk event will occur. This is a user input between 0 and 1.</t>
+      </text>
+    </comment>
+    <comment ref="X2" authorId="14" shapeId="0" xr:uid="{5301FCFF-164C-41C4-AC42-B19C77CCAFCF}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    ID's of the shared uncertainty factors. Keep the ID's in order starting from 1</t>
+      </text>
+    </comment>
+    <comment ref="Y2" authorId="15" shapeId="0" xr:uid="{44C21660-40A7-445E-8543-FF13C2067309}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Description of the shared uncertainity factors. It is not an essential input.
+Uncertainty factors can have an impact on the duration of construction activities. These factors may simultaneously influence multiple activities
+Note that the correlation section is only necessary for the advanced version of the MitC (not the basic)</t>
+      </text>
+    </comment>
+    <comment ref="Z2" authorId="16" shapeId="0" xr:uid="{EFC09581-0698-442A-BCD5-86B53E94AD5B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Duration of the uncertainty factors: three estimates.
+Note that the three estimates must be in ascending order:
+minimum &lt;= Most-likely &lt;= maximum</t>
+      </text>
+    </comment>
+    <comment ref="AC2" authorId="17" shapeId="0" xr:uid="{9BD7A2D3-21C7-4A3A-AB77-E7076CBE9A54}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The ID's of correlated activities that share the uncertainty factor. This is a user input.
+You may insert more than one activity by separating them with a space or a comma.</t>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="18" shapeId="0" xr:uid="{9DA2A3F3-6BD2-494C-AF10-013A710097BC}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is the minimum duration of the activity. The user must define this quantity. 
+To generate random values, you may apply this formula in the cells:
+ =ROUND(RANDBETWEEN(130,160)/100*D7,0)</t>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="19" shapeId="0" xr:uid="{4FE3E174-E4A9-423F-A48D-2D3CF7EF2390}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is the most-likely duration of the activity. The user must define this quantity</t>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="20" shapeId="0" xr:uid="{0C024D35-B30C-499C-8366-794AE12585E6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is the maximum duration of the activity. The user must define this quantity. 
+To generate random values, you may apply this formula in the cells:
+ =ROUND(RANDBETWEEN(130,160)/100*D6,0)</t>
+      </text>
+    </comment>
+    <comment ref="I3" authorId="21" shapeId="0" xr:uid="{9C5512D6-A380-4304-B147-51AFD5410007}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is the minimum (pessimistic) capacity of the mitigation measure. The user must define this quantity.</t>
+      </text>
+    </comment>
+    <comment ref="J3" authorId="22" shapeId="0" xr:uid="{32899173-A5AA-464F-8F9D-EEA5C1D31DBC}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is the most-likely capacity of the mitigation measure. The user must define this quantity.</t>
+      </text>
+    </comment>
+    <comment ref="K3" authorId="23" shapeId="0" xr:uid="{9A9F5103-A2D2-4EE0-BB31-DE11B9398886}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is the maximum (optimistic) capacity of the mitigation measure. The user must define this quantity.</t>
+      </text>
+    </comment>
+    <comment ref="L3" authorId="24" shapeId="0" xr:uid="{36C57516-9BEA-4C79-B2AE-8F26F907B8EE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This factor defines to what extent the mitigation cost variation depends on the mitigation capacity variation. This factor is between 0 and 1. If this factor is set to 1, then the mitigation cost increases/decreases proportionally to the increase/decrease in he mitigation capacity. If it is set to 0, then the cost will remain constant regardless of the variation in the mitigation capacity. You may set any number between 0 and 1 (i.e., 0.5 means partial relation between the cost variation and the mitigation variation)</t>
+      </text>
+    </comment>
+    <comment ref="M3" authorId="25" shapeId="0" xr:uid="{B2442A87-5162-43DD-AF9C-DF7C51A637C3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Minimum cost of the mitigation measure. This is not a user input. It is automatically computed following a predefined formula. To add more cost items to the list, you may copy the formula from any of the cells below.</t>
+      </text>
+    </comment>
+    <comment ref="N3" authorId="26" shapeId="0" xr:uid="{E74F529F-C920-4FFF-AC03-666348C1F3CA}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Most-likely cost of the mitigation measure. This is a user input.</t>
+      </text>
+    </comment>
+    <comment ref="O3" authorId="27" shapeId="0" xr:uid="{4053F11A-ECEF-4B44-9FC5-4B64BAE74102}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Maximum cost of the mitigation measure. This is not a user input. It is automatically computed following a predefined formula. To add more cost items to the list, you may copy the formula from any of the cells below.</t>
+      </text>
+    </comment>
+    <comment ref="S3" authorId="28" shapeId="0" xr:uid="{9E778C37-6EE2-4578-98D4-5BC7AB7B0BB6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is the minimum (optimistic) delay induced by the risk event. The user must define this quantity.</t>
+      </text>
+    </comment>
+    <comment ref="T3" authorId="29" shapeId="0" xr:uid="{D4E34699-714C-43AC-A14F-5B96DF915F7D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is the most-likely delay induced by the risk event. The user must define this quantity.</t>
+      </text>
+    </comment>
+    <comment ref="U3" authorId="30" shapeId="0" xr:uid="{0A841E25-4AE6-4F68-979B-F02C85EF0E9C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is the maximum (pessimistic) delay induced by the risk event. The user must define this quantity.</t>
+      </text>
+    </comment>
+    <comment ref="Z3" authorId="31" shapeId="0" xr:uid="{34521897-0DFC-47DA-9314-BD8C94403FD4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Minimum duration of the uncertainty factor. This is a user input.</t>
+      </text>
+    </comment>
+    <comment ref="AA3" authorId="32" shapeId="0" xr:uid="{7E35FC0E-6F9D-49A4-8589-5906257814F0}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Most-likely duration of the uncertainty factor. This number is to set to 0. We only care about the variation in duration.</t>
+      </text>
+    </comment>
+    <comment ref="AB3" authorId="33" shapeId="0" xr:uid="{EA4240E9-7704-4713-8477-8A0FE2545DE9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Maximum duration of the uncertainty factor. This is a user input.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="106">
   <si>
     <t>Optimistic</t>
-  </si>
-  <si>
-    <t>Likely</t>
   </si>
   <si>
     <t>Pessimistic</t>
@@ -45,28 +376,10 @@
     <t>Most likely</t>
   </si>
   <si>
-    <t>Cost</t>
-  </si>
-  <si>
-    <t>Duration</t>
-  </si>
-  <si>
     <t>maximum</t>
   </si>
   <si>
-    <t>Relationships between measures and activities</t>
-  </si>
-  <si>
     <t>dependency factor (eta)</t>
-  </si>
-  <si>
-    <t>risk event duration</t>
-  </si>
-  <si>
-    <t>Relationships between risk events and activities</t>
-  </si>
-  <si>
-    <t>predecessors</t>
   </si>
   <si>
     <t>18,23,26</t>
@@ -312,31 +625,13 @@
     <t>Mitigation ID</t>
   </si>
   <si>
-    <t>Mitigation duration</t>
-  </si>
-  <si>
-    <t>risk event description</t>
-  </si>
-  <si>
     <t>Risk event ID</t>
-  </si>
-  <si>
-    <t>Shared uncertainty ID</t>
-  </si>
-  <si>
-    <t>Shared uncertainty description</t>
-  </si>
-  <si>
-    <t>correlated activities</t>
   </si>
   <si>
     <t>3,4</t>
   </si>
   <si>
     <t>10,11</t>
-  </si>
-  <si>
-    <t>Durations of Shared activities</t>
   </si>
   <si>
     <t>8,9</t>
@@ -350,12 +645,48 @@
   <si>
     <t>Maximum  (not user input)</t>
   </si>
+  <si>
+    <t>Duration (days)</t>
+  </si>
+  <si>
+    <t>Predecessor activities</t>
+  </si>
+  <si>
+    <t>Mitigation capacity (days)</t>
+  </si>
+  <si>
+    <t>Mitigation cost (euros)</t>
+  </si>
+  <si>
+    <t>Relations with activities</t>
+  </si>
+  <si>
+    <t>Risk event description</t>
+  </si>
+  <si>
+    <t>Risk  duration (days)</t>
+  </si>
+  <si>
+    <t>Affected activities</t>
+  </si>
+  <si>
+    <t>Shared uncertainty factor ID</t>
+  </si>
+  <si>
+    <t>Shared uncertainty factor description</t>
+  </si>
+  <si>
+    <t>Shared uncertainty duration (days)</t>
+  </si>
+  <si>
+    <t>Most-Likely</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -406,6 +737,12 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -678,23 +1015,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -825,94 +1149,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -936,22 +1172,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -960,20 +1180,112 @@
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -991,6 +1303,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1254,12 +1570,138 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A2" dT="2021-07-06T08:54:56.23" personId="{00000000-0000-0000-0000-000000000000}" id="{5EBB22A6-E819-446D-8154-DE25FD7E6A82}">
+    <text>ID's of the activities. Keep the ID's in order starting from 1</text>
+  </threadedComment>
+  <threadedComment ref="B2" dT="2021-07-06T08:55:23.61" personId="{00000000-0000-0000-0000-000000000000}" id="{77119148-1B5B-4125-8F01-307412D847BF}">
+    <text>Description of project activities. It is not an essential input.</text>
+  </threadedComment>
+  <threadedComment ref="C2" dT="2021-07-06T09:11:14.60" personId="{00000000-0000-0000-0000-000000000000}" id="{34228588-1163-43BB-A066-6E6CBEB9DE82}">
+    <text>Activities durations: three estimates
+Note that the three estimates must be in ascending order:
+minimum &lt;= Most-likely &lt;= maximum</text>
+  </threadedComment>
+  <threadedComment ref="F2" dT="2021-07-06T08:53:11.11" personId="{00000000-0000-0000-0000-000000000000}" id="{3166FD02-6A2F-4530-8FE7-452B92D57332}">
+    <text>The ID's of the predecessor activities of each activity. This helps to define dependencies and to generate the project network diagram . This is a user input.
+You may insert more than one predecessor by separating them with a space or a comma</text>
+  </threadedComment>
+  <threadedComment ref="G2" dT="2021-07-06T08:55:55.30" personId="{00000000-0000-0000-0000-000000000000}" id="{498AFDB6-4D70-414D-A23A-477BF3A55DD3}">
+    <text>ID's of the mitigation measures. Keep the ID's in order starting from 1</text>
+  </threadedComment>
+  <threadedComment ref="H2" dT="2021-07-06T08:56:42.79" personId="{00000000-0000-0000-0000-000000000000}" id="{CAE32236-4976-460D-A21C-847ADD9F3F93}">
+    <text>Description of mitigation measures activities. It is not an essential input.</text>
+  </threadedComment>
+  <threadedComment ref="I2" dT="2021-07-06T09:11:38.93" personId="{00000000-0000-0000-0000-000000000000}" id="{76097404-0119-4EF1-8361-CF42159A9F72}">
+    <text>Mitigation capacity of the mitigation measures: three estimates. 
+The mitigation capacity is the duration reduced from the total duration of the influenced activity
+Note that the three estimates must be in ascending order:
+minimum &lt;= Most-likely &lt;= maximum</text>
+  </threadedComment>
+  <threadedComment ref="L2" dT="2021-07-06T09:14:22.89" personId="{00000000-0000-0000-0000-000000000000}" id="{67C32F90-F393-4DFA-B39F-286253EDF727}">
+    <text>Cost of excecuting a mitigation measure</text>
+  </threadedComment>
+  <threadedComment ref="P2" dT="2021-07-06T09:08:52.11" personId="{00000000-0000-0000-0000-000000000000}" id="{A736116B-7089-4E7F-A0FC-748328F3EDED}">
+    <text>The ID's of activities that are influenced by each mitigation measure. 
+One Mitigation measure can influence (i.e., reduce the time of) one or more activities. You may insert more than one activity by separating them with a space or a comma.</text>
+  </threadedComment>
+  <threadedComment ref="Q2" dT="2021-07-06T08:57:34.80" personId="{00000000-0000-0000-0000-000000000000}" id="{B8899479-CE4F-40F6-A0C7-50DAC571D3C4}">
+    <text>ID's of the risk events. Keep the ID's in order starting from 1</text>
+  </threadedComment>
+  <threadedComment ref="R2" dT="2021-07-06T08:56:56.15" personId="{00000000-0000-0000-0000-000000000000}" id="{6CCA99F7-DA14-4459-8FD5-1B0864EF00F8}">
+    <text>Description of risk events. It is not an essential input.</text>
+  </threadedComment>
+  <threadedComment ref="S2" dT="2021-07-06T09:10:36.08" personId="{00000000-0000-0000-0000-000000000000}" id="{EF4EE362-5F89-4AF9-AC3E-CEB75088F726}">
+    <text>The delay induced by each risk event: three estimates.
+Note that the three estimates must be in ascending order:
+minimum &lt;= Most-likely &lt;= maximum</text>
+  </threadedComment>
+  <threadedComment ref="V2" dT="2021-07-06T09:09:01.83" personId="{00000000-0000-0000-0000-000000000000}" id="{CB203497-8043-4A3F-8BBF-A1A90A68AB14}">
+    <text>The ID's of activities that are impacted by each risk event. 
+One risk event can impact (i.e., increase the time of) one or more activities. You may insert more than one activity by separating them with a space or a comma.</text>
+  </threadedComment>
+  <threadedComment ref="W2" dT="2021-07-06T09:17:27.88" personId="{00000000-0000-0000-0000-000000000000}" id="{B50C9B52-DF4C-4A39-8A57-0D501A9882F9}">
+    <text>This is the probability that a risk event will occur. This is a user input between 0 and 1.</text>
+  </threadedComment>
+  <threadedComment ref="X2" dT="2021-07-06T08:57:49.90" personId="{00000000-0000-0000-0000-000000000000}" id="{5301FCFF-164C-41C4-AC42-B19C77CCAFCF}">
+    <text>ID's of the shared uncertainty factors. Keep the ID's in order starting from 1</text>
+  </threadedComment>
+  <threadedComment ref="Y2" dT="2021-07-06T08:57:15.26" personId="{00000000-0000-0000-0000-000000000000}" id="{44C21660-40A7-445E-8543-FF13C2067309}">
+    <text>Description of the shared uncertainity factors. It is not an essential input.
+Uncertainty factors can have an impact on the duration of construction activities. These factors may simultaneously influence multiple activities
+Note that the correlation section is only necessary for the advanced version of the MitC (not the basic)</text>
+  </threadedComment>
+  <threadedComment ref="Z2" dT="2021-07-06T09:19:29.68" personId="{00000000-0000-0000-0000-000000000000}" id="{EFC09581-0698-442A-BCD5-86B53E94AD5B}">
+    <text>Duration of the uncertainty factors: three estimates.
+Note that the three estimates must be in ascending order:
+minimum &lt;= Most-likely &lt;= maximum</text>
+  </threadedComment>
+  <threadedComment ref="AC2" dT="2021-07-06T09:24:56.05" personId="{00000000-0000-0000-0000-000000000000}" id="{9BD7A2D3-21C7-4A3A-AB77-E7076CBE9A54}">
+    <text>The ID's of correlated activities that share the uncertainty factor. This is a user input.
+You may insert more than one activity by separating them with a space or a comma.</text>
+  </threadedComment>
+  <threadedComment ref="C3" dT="2021-03-17T15:19:05.26" personId="{00000000-0000-0000-0000-000000000000}" id="{9DA2A3F3-6BD2-494C-AF10-013A710097BC}">
+    <text>This is the minimum duration of the activity. The user must define this quantity. 
+To generate random values, you may apply this formula in the cells:
+ =ROUND(RANDBETWEEN(130,160)/100*D7,0)</text>
+  </threadedComment>
+  <threadedComment ref="D3" dT="2021-07-06T08:49:12.47" personId="{00000000-0000-0000-0000-000000000000}" id="{4FE3E174-E4A9-423F-A48D-2D3CF7EF2390}">
+    <text>This is the most-likely duration of the activity. The user must define this quantity</text>
+  </threadedComment>
+  <threadedComment ref="E3" dT="2021-03-17T15:19:15.46" personId="{00000000-0000-0000-0000-000000000000}" id="{0C024D35-B30C-499C-8366-794AE12585E6}">
+    <text>This is the maximum duration of the activity. The user must define this quantity. 
+To generate random values, you may apply this formula in the cells:
+ =ROUND(RANDBETWEEN(130,160)/100*D6,0)</text>
+  </threadedComment>
+  <threadedComment ref="I3" dT="2021-07-06T08:58:44.60" personId="{00000000-0000-0000-0000-000000000000}" id="{9C5512D6-A380-4304-B147-51AFD5410007}">
+    <text>This is the minimum (pessimistic) capacity of the mitigation measure. The user must define this quantity.</text>
+  </threadedComment>
+  <threadedComment ref="J3" dT="2021-07-06T08:59:04.11" personId="{00000000-0000-0000-0000-000000000000}" id="{32899173-A5AA-464F-8F9D-EEA5C1D31DBC}">
+    <text>This is the most-likely capacity of the mitigation measure. The user must define this quantity.</text>
+  </threadedComment>
+  <threadedComment ref="K3" dT="2021-07-06T08:58:51.76" personId="{00000000-0000-0000-0000-000000000000}" id="{9A9F5103-A2D2-4EE0-BB31-DE11B9398886}">
+    <text>This is the maximum (optimistic) capacity of the mitigation measure. The user must define this quantity.</text>
+  </threadedComment>
+  <threadedComment ref="L3" dT="2021-07-06T09:01:51.41" personId="{00000000-0000-0000-0000-000000000000}" id="{36C57516-9BEA-4C79-B2AE-8F26F907B8EE}">
+    <text>This factor defines to what extent the mitigation cost variation depends on the mitigation capacity variation. This factor is between 0 and 1. If this factor is set to 1, then the mitigation cost increases/decreases proportionally to the increase/decrease in he mitigation capacity. If it is set to 0, then the cost will remain constant regardless of the variation in the mitigation capacity. You may set any number between 0 and 1 (i.e., 0.5 means partial relation between the cost variation and the mitigation variation)</text>
+  </threadedComment>
+  <threadedComment ref="M3" dT="2021-07-06T09:05:49.65" personId="{00000000-0000-0000-0000-000000000000}" id="{B2442A87-5162-43DD-AF9C-DF7C51A637C3}">
+    <text>Minimum cost of the mitigation measure. This is not a user input. It is automatically computed following a predefined formula. To add more cost items to the list, you may copy the formula from any of the cells below.</text>
+  </threadedComment>
+  <threadedComment ref="N3" dT="2021-07-06T09:06:08.20" personId="{00000000-0000-0000-0000-000000000000}" id="{E74F529F-C920-4FFF-AC03-666348C1F3CA}">
+    <text>Most-likely cost of the mitigation measure. This is a user input.</text>
+  </threadedComment>
+  <threadedComment ref="O3" dT="2021-07-06T09:07:02.57" personId="{00000000-0000-0000-0000-000000000000}" id="{4053F11A-ECEF-4B44-9FC5-4B64BAE74102}">
+    <text>Maximum cost of the mitigation measure. This is not a user input. It is automatically computed following a predefined formula. To add more cost items to the list, you may copy the formula from any of the cells below.</text>
+  </threadedComment>
+  <threadedComment ref="S3" dT="2021-07-06T09:15:48.93" personId="{00000000-0000-0000-0000-000000000000}" id="{9E778C37-6EE2-4578-98D4-5BC7AB7B0BB6}">
+    <text>This is the minimum (optimistic) delay induced by the risk event. The user must define this quantity.</text>
+  </threadedComment>
+  <threadedComment ref="T3" dT="2021-07-06T09:16:10.31" personId="{00000000-0000-0000-0000-000000000000}" id="{D4E34699-714C-43AC-A14F-5B96DF915F7D}">
+    <text>This is the most-likely delay induced by the risk event. The user must define this quantity.</text>
+  </threadedComment>
+  <threadedComment ref="U3" dT="2021-07-06T09:16:02.73" personId="{00000000-0000-0000-0000-000000000000}" id="{0A841E25-4AE6-4F68-979B-F02C85EF0E9C}">
+    <text>This is the maximum (pessimistic) delay induced by the risk event. The user must define this quantity.</text>
+  </threadedComment>
+  <threadedComment ref="Z3" dT="2021-07-06T09:23:43.35" personId="{00000000-0000-0000-0000-000000000000}" id="{34521897-0DFC-47DA-9314-BD8C94403FD4}">
+    <text>Minimum duration of the uncertainty factor. This is a user input.</text>
+  </threadedComment>
+  <threadedComment ref="AA3" dT="2021-07-06T09:24:33.90" personId="{00000000-0000-0000-0000-000000000000}" id="{7E35FC0E-6F9D-49A4-8589-5906257814F0}">
+    <text>Most-likely duration of the uncertainty factor. This number is to set to 0. We only care about the variation in duration.</text>
+  </threadedComment>
+  <threadedComment ref="AB3" dT="2021-07-06T09:24:44.31" personId="{00000000-0000-0000-0000-000000000000}" id="{EA4240E9-7704-4713-8477-8A0FE2545DE9}">
+    <text>Maximum duration of the uncertainty factor. This is a user input.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC8281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R29" sqref="R29"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1293,23 +1735,23 @@
     <col min="30" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="69">
+    <row r="1" spans="1:29" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="43">
         <v>1</v>
       </c>
-      <c r="B1" s="70">
+      <c r="B1" s="44">
         <v>2</v>
       </c>
-      <c r="C1" s="70">
+      <c r="C1" s="44">
         <v>3</v>
       </c>
-      <c r="D1" s="70">
+      <c r="D1" s="44">
         <v>4</v>
       </c>
-      <c r="E1" s="70">
+      <c r="E1" s="44">
         <v>5</v>
       </c>
-      <c r="F1" s="71">
+      <c r="F1" s="45">
         <v>6</v>
       </c>
       <c r="G1" s="2">
@@ -1382,2371 +1824,2371 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="72" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="73" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2" s="73" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="74" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="60" t="s">
-        <v>93</v>
-      </c>
-      <c r="H2" s="58" t="s">
-        <v>92</v>
+    <row r="2" spans="1:29" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="54" t="s">
+        <v>85</v>
       </c>
       <c r="I2" s="54" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J2" s="54"/>
       <c r="K2" s="54"/>
       <c r="L2" s="54" t="s">
-        <v>5</v>
+        <v>97</v>
       </c>
       <c r="M2" s="54"/>
       <c r="N2" s="54"/>
       <c r="O2" s="54"/>
-      <c r="P2" s="52" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q2" s="63" t="s">
-        <v>96</v>
-      </c>
-      <c r="R2" s="55" t="s">
-        <v>95</v>
-      </c>
-      <c r="S2" s="48" t="s">
+      <c r="P2" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q2" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="R2" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="S2" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
+      <c r="V2" s="57" t="s">
+        <v>101</v>
+      </c>
+      <c r="W2" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="X2" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y2" s="59" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z2" s="59" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA2" s="59"/>
+      <c r="AB2" s="59"/>
+      <c r="AC2" s="59" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" s="60" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="61"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="63" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="63" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="64"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="67" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="67" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" s="67" t="s">
+        <v>92</v>
+      </c>
+      <c r="N3" s="67" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" s="67" t="s">
+        <v>93</v>
+      </c>
+      <c r="P3" s="68"/>
+      <c r="Q3" s="69"/>
+      <c r="R3" s="70"/>
+      <c r="S3" s="71" t="s">
+        <v>2</v>
+      </c>
+      <c r="T3" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="U3" s="71" t="s">
+        <v>4</v>
+      </c>
+      <c r="V3" s="70"/>
+      <c r="W3" s="70"/>
+      <c r="X3" s="72"/>
+      <c r="Y3" s="73"/>
+      <c r="Z3" s="74" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA3" s="74" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB3" s="74" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC3" s="73"/>
+    </row>
+    <row r="4" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="T2" s="48"/>
-      <c r="U2" s="48"/>
-      <c r="V2" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="W2" s="50" t="s">
-        <v>72</v>
-      </c>
-      <c r="X2" s="43" t="s">
-        <v>97</v>
-      </c>
-      <c r="Y2" s="45" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z2" s="47" t="s">
-        <v>102</v>
-      </c>
-      <c r="AA2" s="47"/>
-      <c r="AB2" s="47"/>
-      <c r="AC2" s="78" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="57"/>
-      <c r="B3" s="62"/>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="5">
         <v>0</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="46"/>
+      <c r="G4" s="7">
         <v>1</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="75"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="56"/>
-      <c r="S3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="V3" s="49"/>
-      <c r="W3" s="51"/>
-      <c r="X3" s="44"/>
-      <c r="Y3" s="46"/>
-      <c r="Z3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC3" s="79"/>
-    </row>
-    <row r="4" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
-        <v>1</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="9">
-        <v>0</v>
-      </c>
-      <c r="D4" s="10">
-        <v>0</v>
-      </c>
-      <c r="E4" s="9">
-        <v>0</v>
-      </c>
-      <c r="F4" s="76"/>
-      <c r="G4" s="11">
-        <v>1</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="I4" s="9">
+      <c r="H4" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="5">
         <v>51</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="9">
         <v>52</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="5">
         <v>52</v>
       </c>
-      <c r="L4" s="14">
+      <c r="L4" s="10">
         <v>0.5</v>
       </c>
-      <c r="M4" s="41">
+      <c r="M4" s="37">
         <f>N4*(1-(L4*(J4-I4)/J4))</f>
         <v>118846.15384615384</v>
       </c>
-      <c r="N4" s="15">
+      <c r="N4" s="11">
         <v>120000</v>
       </c>
-      <c r="O4" s="41">
+      <c r="O4" s="37">
         <f>N4*(1-(L4*(J4-K4)/J4))</f>
         <v>120000</v>
       </c>
-      <c r="P4" s="16">
+      <c r="P4" s="12">
         <v>3</v>
       </c>
-      <c r="Q4" s="17">
+      <c r="Q4" s="13">
         <v>1</v>
       </c>
-      <c r="R4" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="S4" s="14">
+      <c r="R4" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="S4" s="10">
         <v>96</v>
       </c>
-      <c r="T4" s="18">
+      <c r="T4" s="14">
         <v>105</v>
       </c>
-      <c r="U4" s="14">
+      <c r="U4" s="10">
         <v>119</v>
       </c>
-      <c r="V4" s="14">
+      <c r="V4" s="10">
         <v>3</v>
       </c>
-      <c r="W4" s="19">
+      <c r="W4" s="15">
         <v>0.2</v>
       </c>
-      <c r="X4" s="20">
+      <c r="X4" s="16">
         <v>1</v>
       </c>
-      <c r="Y4" s="12"/>
-      <c r="Z4" s="9">
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="5">
         <v>120</v>
       </c>
-      <c r="AA4" s="12">
+      <c r="AA4" s="8">
         <v>121</v>
       </c>
-      <c r="AB4" s="9">
+      <c r="AB4" s="5">
         <v>154</v>
       </c>
-      <c r="AC4" s="80" t="s">
-        <v>100</v>
+      <c r="AC4" s="48" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="A5" s="3">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="9">
+      <c r="B5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="5">
         <v>0</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="6">
         <v>0</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="5">
         <v>0</v>
       </c>
-      <c r="F5" s="76"/>
-      <c r="G5" s="11">
+      <c r="F5" s="46"/>
+      <c r="G5" s="7">
         <v>2</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="I5" s="9">
+      <c r="H5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="5">
         <v>7</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="9">
         <v>7</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="5">
         <v>7</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="10">
         <v>0.5</v>
       </c>
-      <c r="M5" s="41">
+      <c r="M5" s="37">
         <f t="shared" ref="M5:M22" si="0">N5*(1-(L5*(J5-I5)/J5))</f>
         <v>30000</v>
       </c>
-      <c r="N5" s="15">
+      <c r="N5" s="11">
         <v>30000</v>
       </c>
-      <c r="O5" s="41">
+      <c r="O5" s="37">
         <f t="shared" ref="O5:O22" si="1">N5*(1-(L5*(J5-K5)/J5))</f>
         <v>30000</v>
       </c>
-      <c r="P5" s="16">
+      <c r="P5" s="12">
         <v>4</v>
       </c>
-      <c r="Q5" s="17">
+      <c r="Q5" s="13">
         <v>2</v>
       </c>
-      <c r="R5" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="S5" s="14">
+      <c r="R5" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="S5" s="10">
         <v>13</v>
       </c>
-      <c r="T5" s="18">
+      <c r="T5" s="14">
         <v>14</v>
       </c>
-      <c r="U5" s="14">
+      <c r="U5" s="10">
         <v>15</v>
       </c>
-      <c r="V5" s="14">
+      <c r="V5" s="10">
         <v>4</v>
       </c>
-      <c r="W5" s="19">
+      <c r="W5" s="15">
         <v>0.05</v>
       </c>
-      <c r="X5" s="20">
+      <c r="X5" s="16">
         <v>2</v>
       </c>
-      <c r="Y5" s="12"/>
-      <c r="Z5" s="9">
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="5">
         <v>180</v>
       </c>
-      <c r="AA5" s="12">
+      <c r="AA5" s="8">
         <v>190</v>
       </c>
-      <c r="AB5" s="9">
+      <c r="AB5" s="5">
         <v>240</v>
       </c>
-      <c r="AC5" s="80" t="s">
-        <v>103</v>
+      <c r="AC5" s="48" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="A6" s="3">
         <v>3</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="9">
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5">
         <v>865</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="6">
         <v>920</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="5">
         <v>1040</v>
       </c>
-      <c r="F6" s="32">
+      <c r="F6" s="28">
         <v>1</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="7">
         <v>3</v>
       </c>
-      <c r="H6" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="I6" s="9">
+      <c r="H6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="5">
         <v>53</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="9">
         <v>65</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="5">
         <v>65</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="10">
         <v>0.5</v>
       </c>
-      <c r="M6" s="41">
+      <c r="M6" s="37">
         <f t="shared" si="0"/>
         <v>136153.84615384616</v>
       </c>
-      <c r="N6" s="15">
+      <c r="N6" s="11">
         <v>150000</v>
       </c>
-      <c r="O6" s="41">
+      <c r="O6" s="37">
         <f t="shared" si="1"/>
         <v>150000</v>
       </c>
-      <c r="P6" s="16">
+      <c r="P6" s="12">
         <v>7</v>
       </c>
-      <c r="Q6" s="17">
+      <c r="Q6" s="13">
         <v>3</v>
       </c>
-      <c r="R6" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="S6" s="14">
+      <c r="R6" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="S6" s="10">
         <v>63</v>
       </c>
-      <c r="T6" s="18">
+      <c r="T6" s="14">
         <v>70</v>
       </c>
-      <c r="U6" s="14">
+      <c r="U6" s="10">
         <v>78</v>
       </c>
-      <c r="V6" s="14">
+      <c r="V6" s="10">
         <v>7</v>
       </c>
-      <c r="W6" s="19">
+      <c r="W6" s="15">
         <v>0.15</v>
       </c>
-      <c r="X6" s="20">
+      <c r="X6" s="16">
         <v>3</v>
       </c>
-      <c r="Y6" s="12"/>
-      <c r="Z6" s="9">
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="5">
         <v>225</v>
       </c>
-      <c r="AA6" s="12">
+      <c r="AA6" s="8">
         <v>250</v>
       </c>
-      <c r="AB6" s="9">
+      <c r="AB6" s="5">
         <v>310</v>
       </c>
-      <c r="AC6" s="80" t="s">
-        <v>101</v>
+      <c r="AC6" s="48" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="A7" s="3">
         <v>4</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="9">
+      <c r="B7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="5">
         <v>128</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="6">
         <v>130</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="5">
         <v>164</v>
       </c>
-      <c r="F7" s="32">
+      <c r="F7" s="28">
         <v>1</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="7">
         <v>4</v>
       </c>
-      <c r="H7" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="I7" s="9">
+      <c r="H7" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="5">
         <v>22</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="9">
         <v>26</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K7" s="5">
         <v>29</v>
       </c>
-      <c r="L7" s="14">
+      <c r="L7" s="10">
         <v>0.5</v>
       </c>
-      <c r="M7" s="41">
+      <c r="M7" s="37">
         <f t="shared" si="0"/>
         <v>44307.692307692312</v>
       </c>
-      <c r="N7" s="15">
+      <c r="N7" s="11">
         <v>48000</v>
       </c>
-      <c r="O7" s="41">
+      <c r="O7" s="37">
         <f t="shared" si="1"/>
         <v>50769.230769230773</v>
       </c>
-      <c r="P7" s="16">
+      <c r="P7" s="12">
         <v>8</v>
       </c>
-      <c r="Q7" s="17">
+      <c r="Q7" s="13">
         <v>4</v>
       </c>
-      <c r="R7" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="S7" s="14">
+      <c r="R7" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="S7" s="10">
         <v>35</v>
       </c>
-      <c r="T7" s="18">
+      <c r="T7" s="14">
         <v>35</v>
       </c>
-      <c r="U7" s="14">
+      <c r="U7" s="10">
         <v>41</v>
       </c>
-      <c r="V7" s="14">
+      <c r="V7" s="10">
         <v>8</v>
       </c>
-      <c r="W7" s="19">
+      <c r="W7" s="15">
         <v>0.2</v>
       </c>
-      <c r="X7" s="20">
+      <c r="X7" s="16">
         <v>4</v>
       </c>
-      <c r="Y7" s="12"/>
-      <c r="Z7" s="9">
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="5">
         <v>148</v>
       </c>
-      <c r="AA7" s="12">
+      <c r="AA7" s="8">
         <v>155</v>
       </c>
-      <c r="AB7" s="9">
+      <c r="AB7" s="5">
         <v>170</v>
       </c>
-      <c r="AC7" s="80" t="s">
-        <v>104</v>
+      <c r="AC7" s="48" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="A8" s="3">
         <v>5</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="9">
+      <c r="B8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="5">
         <v>0</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="6">
         <v>0</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="5">
         <v>0</v>
       </c>
-      <c r="F8" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="11">
+      <c r="F8" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="7">
         <v>5</v>
       </c>
-      <c r="H8" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="I8" s="9">
+      <c r="H8" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="5">
         <v>21</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="9">
         <v>26</v>
       </c>
-      <c r="K8" s="9">
+      <c r="K8" s="5">
         <v>26</v>
       </c>
-      <c r="L8" s="14">
+      <c r="L8" s="10">
         <v>0.5</v>
       </c>
-      <c r="M8" s="41">
+      <c r="M8" s="37">
         <f t="shared" si="0"/>
         <v>677884.61538461538</v>
       </c>
-      <c r="N8" s="15">
+      <c r="N8" s="11">
         <v>750000</v>
       </c>
-      <c r="O8" s="41">
+      <c r="O8" s="37">
         <f t="shared" si="1"/>
         <v>750000</v>
       </c>
-      <c r="P8" s="16">
+      <c r="P8" s="12">
         <v>9</v>
       </c>
-      <c r="Q8" s="17">
+      <c r="Q8" s="13">
         <v>5</v>
       </c>
-      <c r="R8" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="S8" s="14">
+      <c r="R8" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="S8" s="10">
         <v>34</v>
       </c>
-      <c r="T8" s="18">
+      <c r="T8" s="14">
         <v>35</v>
       </c>
-      <c r="U8" s="14">
+      <c r="U8" s="10">
         <v>40</v>
       </c>
-      <c r="V8" s="14">
+      <c r="V8" s="10">
         <v>9</v>
       </c>
-      <c r="W8" s="19">
+      <c r="W8" s="15">
         <v>0.1</v>
       </c>
-      <c r="X8" s="20"/>
-      <c r="Y8" s="12"/>
-      <c r="Z8" s="9"/>
-      <c r="AA8" s="12"/>
-      <c r="AB8" s="9"/>
-      <c r="AC8" s="80"/>
+      <c r="X8" s="16"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="5"/>
+      <c r="AC8" s="48"/>
     </row>
     <row r="9" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+      <c r="A9" s="3">
         <v>6</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="9">
+      <c r="B9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="5">
         <v>0</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="6">
         <v>0</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="5">
         <v>0</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F9" s="28">
         <v>5</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="7">
         <v>6</v>
       </c>
-      <c r="H9" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="I9" s="9">
+      <c r="H9" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I9" s="5">
         <v>47</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="9">
         <v>52</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="5">
         <v>55</v>
       </c>
-      <c r="L9" s="14">
+      <c r="L9" s="10">
         <v>0.5</v>
       </c>
-      <c r="M9" s="41">
+      <c r="M9" s="37">
         <f t="shared" si="0"/>
         <v>190384.61538461538</v>
       </c>
-      <c r="N9" s="15">
+      <c r="N9" s="11">
         <v>200000</v>
       </c>
-      <c r="O9" s="41">
+      <c r="O9" s="37">
         <f t="shared" si="1"/>
         <v>205769.23076923075</v>
       </c>
-      <c r="P9" s="16">
+      <c r="P9" s="12">
         <v>10</v>
       </c>
-      <c r="Q9" s="17">
+      <c r="Q9" s="13">
         <v>6</v>
       </c>
-      <c r="R9" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="S9" s="14">
+      <c r="R9" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="S9" s="10">
         <v>14</v>
       </c>
-      <c r="T9" s="18">
+      <c r="T9" s="14">
         <v>14</v>
       </c>
-      <c r="U9" s="14">
+      <c r="U9" s="10">
         <v>15</v>
       </c>
-      <c r="V9" s="14">
+      <c r="V9" s="10">
         <v>10</v>
       </c>
-      <c r="W9" s="19">
+      <c r="W9" s="15">
         <v>0.1</v>
       </c>
-      <c r="X9" s="20"/>
-      <c r="Y9" s="12"/>
-      <c r="Z9" s="9"/>
-      <c r="AA9" s="12"/>
-      <c r="AB9" s="9"/>
-      <c r="AC9" s="80"/>
+      <c r="X9" s="16"/>
+      <c r="Y9" s="8"/>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="5"/>
+      <c r="AC9" s="48"/>
     </row>
     <row r="10" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="3">
         <v>7</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="9">
+      <c r="B10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="5">
         <v>1194</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="6">
         <v>1284</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="5">
         <v>1541</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="28">
         <v>6</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="7">
         <v>7</v>
       </c>
-      <c r="H10" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="I10" s="9">
+      <c r="H10" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="5">
         <v>60</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="9">
         <v>65</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="5">
         <v>66</v>
       </c>
-      <c r="L10" s="14">
+      <c r="L10" s="10">
         <v>0.5</v>
       </c>
-      <c r="M10" s="41">
+      <c r="M10" s="37">
         <f t="shared" si="0"/>
         <v>144230.76923076925</v>
       </c>
-      <c r="N10" s="15">
+      <c r="N10" s="11">
         <v>150000</v>
       </c>
-      <c r="O10" s="41">
+      <c r="O10" s="37">
         <f t="shared" si="1"/>
         <v>151153.84615384616</v>
       </c>
-      <c r="P10" s="16">
+      <c r="P10" s="12">
         <v>11</v>
       </c>
-      <c r="Q10" s="17">
+      <c r="Q10" s="13">
         <v>7</v>
       </c>
-      <c r="R10" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="S10" s="14">
+      <c r="R10" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="S10" s="10">
         <v>19</v>
       </c>
-      <c r="T10" s="18">
+      <c r="T10" s="14">
         <v>21</v>
       </c>
-      <c r="U10" s="14">
+      <c r="U10" s="10">
         <v>25</v>
       </c>
-      <c r="V10" s="14">
+      <c r="V10" s="10">
         <v>11</v>
       </c>
-      <c r="W10" s="19">
+      <c r="W10" s="15">
         <v>0.2</v>
       </c>
-      <c r="X10" s="20"/>
-      <c r="Y10" s="12"/>
-      <c r="Z10" s="9"/>
-      <c r="AA10" s="12"/>
-      <c r="AB10" s="9"/>
-      <c r="AC10" s="80"/>
+      <c r="X10" s="16"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="8"/>
+      <c r="AB10" s="5"/>
+      <c r="AC10" s="48"/>
     </row>
     <row r="11" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="A11" s="3">
         <v>8</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="9">
+      <c r="B11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="5">
         <v>182</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="6">
         <v>200</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="5">
         <v>256</v>
       </c>
-      <c r="F11" s="32">
+      <c r="F11" s="28">
         <v>6</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="7">
         <v>8</v>
       </c>
-      <c r="H11" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="I11" s="9">
+      <c r="H11" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="5">
         <v>26</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="9">
         <v>26</v>
       </c>
-      <c r="K11" s="9">
+      <c r="K11" s="5">
         <v>26</v>
       </c>
-      <c r="L11" s="14">
+      <c r="L11" s="10">
         <v>0.5</v>
       </c>
-      <c r="M11" s="41">
+      <c r="M11" s="37">
         <f t="shared" si="0"/>
         <v>60000</v>
       </c>
-      <c r="N11" s="15">
+      <c r="N11" s="11">
         <v>60000</v>
       </c>
-      <c r="O11" s="41">
+      <c r="O11" s="37">
         <f t="shared" si="1"/>
         <v>60000</v>
       </c>
-      <c r="P11" s="16">
+      <c r="P11" s="12">
         <v>12</v>
       </c>
-      <c r="Q11" s="17">
+      <c r="Q11" s="13">
         <v>8</v>
       </c>
-      <c r="R11" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="S11" s="14">
+      <c r="R11" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="S11" s="10">
         <v>20</v>
       </c>
-      <c r="T11" s="18">
+      <c r="T11" s="14">
         <v>21</v>
       </c>
-      <c r="U11" s="14">
+      <c r="U11" s="10">
         <v>22</v>
       </c>
-      <c r="V11" s="14">
+      <c r="V11" s="10">
         <v>12</v>
       </c>
-      <c r="W11" s="19">
+      <c r="W11" s="15">
         <v>0.25</v>
       </c>
-      <c r="X11" s="20"/>
-      <c r="Y11" s="12"/>
-      <c r="Z11" s="9"/>
-      <c r="AA11" s="12"/>
-      <c r="AB11" s="9"/>
-      <c r="AC11" s="80"/>
+      <c r="X11" s="16"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="5"/>
+      <c r="AC11" s="48"/>
     </row>
     <row r="12" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="A12" s="3">
         <v>9</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="9">
+      <c r="B12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="5">
         <v>363</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="6">
         <v>395</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="5">
         <v>486</v>
       </c>
-      <c r="F12" s="32">
+      <c r="F12" s="28">
         <v>6</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="7">
         <v>9</v>
       </c>
-      <c r="H12" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="I12" s="9">
+      <c r="H12" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="5">
         <v>27</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="9">
         <v>33</v>
       </c>
-      <c r="K12" s="9">
+      <c r="K12" s="5">
         <v>33</v>
       </c>
-      <c r="L12" s="14">
+      <c r="L12" s="10">
         <v>0.5</v>
       </c>
-      <c r="M12" s="41">
+      <c r="M12" s="37">
         <f t="shared" si="0"/>
         <v>90909.090909090912</v>
       </c>
-      <c r="N12" s="15">
+      <c r="N12" s="11">
         <v>100000</v>
       </c>
-      <c r="O12" s="41">
+      <c r="O12" s="37">
         <f t="shared" si="1"/>
         <v>100000</v>
       </c>
-      <c r="P12" s="16">
+      <c r="P12" s="12">
         <v>14</v>
       </c>
-      <c r="Q12" s="17">
+      <c r="Q12" s="13">
         <v>9</v>
       </c>
-      <c r="R12" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="S12" s="14">
+      <c r="R12" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="S12" s="10">
         <v>20</v>
       </c>
-      <c r="T12" s="18">
+      <c r="T12" s="14">
         <v>21</v>
       </c>
-      <c r="U12" s="14">
+      <c r="U12" s="10">
         <v>23</v>
       </c>
-      <c r="V12" s="14">
+      <c r="V12" s="10">
         <v>14</v>
       </c>
-      <c r="W12" s="19">
+      <c r="W12" s="15">
         <v>0.05</v>
       </c>
-      <c r="X12" s="20"/>
-      <c r="Y12" s="12"/>
-      <c r="Z12" s="9"/>
-      <c r="AA12" s="12"/>
-      <c r="AB12" s="9"/>
-      <c r="AC12" s="80"/>
+      <c r="X12" s="16"/>
+      <c r="Y12" s="8"/>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="8"/>
+      <c r="AB12" s="5"/>
+      <c r="AC12" s="48"/>
     </row>
     <row r="13" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+      <c r="A13" s="3">
         <v>10</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="9">
+      <c r="B13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="5">
         <v>234</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="6">
         <v>260</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="5">
         <v>325</v>
       </c>
-      <c r="F13" s="32">
+      <c r="F13" s="28">
         <v>6</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="7">
         <v>10</v>
       </c>
-      <c r="H13" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="I13" s="9">
+      <c r="H13" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I13" s="5">
         <v>23</v>
       </c>
-      <c r="J13" s="13">
+      <c r="J13" s="9">
         <v>26</v>
       </c>
-      <c r="K13" s="9">
+      <c r="K13" s="5">
         <v>27</v>
       </c>
-      <c r="L13" s="14">
+      <c r="L13" s="10">
         <v>0.5</v>
       </c>
-      <c r="M13" s="41">
+      <c r="M13" s="37">
         <f t="shared" si="0"/>
         <v>235576.92307692306</v>
       </c>
-      <c r="N13" s="15">
+      <c r="N13" s="11">
         <v>250000</v>
       </c>
-      <c r="O13" s="41">
+      <c r="O13" s="37">
         <f t="shared" si="1"/>
         <v>254807.69230769228</v>
       </c>
-      <c r="P13" s="16">
+      <c r="P13" s="12">
         <v>15</v>
       </c>
-      <c r="Q13" s="17">
+      <c r="Q13" s="13">
         <v>10</v>
       </c>
-      <c r="R13" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="S13" s="14">
+      <c r="R13" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="S13" s="10">
         <v>13</v>
       </c>
-      <c r="T13" s="18">
+      <c r="T13" s="14">
         <v>14</v>
       </c>
-      <c r="U13" s="14">
+      <c r="U13" s="10">
         <v>15</v>
       </c>
-      <c r="V13" s="14">
+      <c r="V13" s="10">
         <v>15</v>
       </c>
-      <c r="W13" s="19">
+      <c r="W13" s="15">
         <v>0.05</v>
       </c>
-      <c r="X13" s="20"/>
-      <c r="Y13" s="12"/>
-      <c r="Z13" s="9"/>
-      <c r="AA13" s="12"/>
-      <c r="AB13" s="9"/>
-      <c r="AC13" s="80"/>
+      <c r="X13" s="16"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="8"/>
+      <c r="AB13" s="5"/>
+      <c r="AC13" s="48"/>
     </row>
     <row r="14" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+      <c r="A14" s="3">
         <v>11</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="9">
+      <c r="B14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="5">
         <v>305</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="6">
         <v>335</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="5">
         <v>425</v>
       </c>
-      <c r="F14" s="32">
+      <c r="F14" s="28">
         <v>6</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="7">
         <v>11</v>
       </c>
-      <c r="H14" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="I14" s="9">
+      <c r="H14" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" s="5">
         <v>103</v>
       </c>
-      <c r="J14" s="13">
+      <c r="J14" s="9">
         <v>104</v>
       </c>
-      <c r="K14" s="9">
+      <c r="K14" s="5">
         <v>114</v>
       </c>
-      <c r="L14" s="14">
+      <c r="L14" s="10">
         <v>0.5</v>
       </c>
-      <c r="M14" s="41">
+      <c r="M14" s="37">
         <f t="shared" si="0"/>
         <v>199038.46153846153</v>
       </c>
-      <c r="N14" s="15">
+      <c r="N14" s="11">
         <v>200000</v>
       </c>
-      <c r="O14" s="41">
+      <c r="O14" s="37">
         <f t="shared" si="1"/>
         <v>209615.38461538462</v>
       </c>
-      <c r="P14" s="16">
+      <c r="P14" s="12">
         <v>16</v>
       </c>
-      <c r="Q14" s="17">
+      <c r="Q14" s="13">
         <v>11</v>
       </c>
-      <c r="R14" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="S14" s="14">
+      <c r="R14" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="S14" s="10">
         <v>33</v>
       </c>
-      <c r="T14" s="18">
+      <c r="T14" s="14">
         <v>35</v>
       </c>
-      <c r="U14" s="14">
+      <c r="U14" s="10">
         <v>41</v>
       </c>
-      <c r="V14" s="14">
+      <c r="V14" s="10">
         <v>16</v>
       </c>
-      <c r="W14" s="19">
+      <c r="W14" s="15">
         <v>0.1</v>
       </c>
-      <c r="X14" s="20"/>
-      <c r="Y14" s="12"/>
-      <c r="Z14" s="9"/>
-      <c r="AA14" s="12"/>
-      <c r="AB14" s="9"/>
-      <c r="AC14" s="80"/>
+      <c r="X14" s="16"/>
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="8"/>
+      <c r="AB14" s="5"/>
+      <c r="AC14" s="48"/>
     </row>
     <row r="15" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+      <c r="A15" s="3">
         <v>12</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="9">
+      <c r="B15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="5">
         <v>120</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="6">
         <v>128</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="5">
         <v>155</v>
       </c>
-      <c r="F15" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="11">
+      <c r="F15" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="7">
         <v>12</v>
       </c>
-      <c r="H15" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="I15" s="9">
+      <c r="H15" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="I15" s="5">
         <v>7</v>
       </c>
-      <c r="J15" s="13">
+      <c r="J15" s="9">
         <v>7</v>
       </c>
-      <c r="K15" s="9">
+      <c r="K15" s="5">
         <v>7</v>
       </c>
-      <c r="L15" s="14">
+      <c r="L15" s="10">
         <v>0.5</v>
       </c>
-      <c r="M15" s="41">
+      <c r="M15" s="37">
         <f t="shared" si="0"/>
         <v>30000</v>
       </c>
-      <c r="N15" s="15">
+      <c r="N15" s="11">
         <v>30000</v>
       </c>
-      <c r="O15" s="41">
+      <c r="O15" s="37">
         <f t="shared" si="1"/>
         <v>30000</v>
       </c>
-      <c r="P15" s="16">
+      <c r="P15" s="12">
         <v>18</v>
       </c>
-      <c r="Q15" s="17">
+      <c r="Q15" s="13">
         <v>12</v>
       </c>
-      <c r="R15" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="S15" s="14">
+      <c r="R15" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="S15" s="10">
         <v>20</v>
       </c>
-      <c r="T15" s="18">
+      <c r="T15" s="14">
         <v>21</v>
       </c>
-      <c r="U15" s="14">
+      <c r="U15" s="10">
         <v>21</v>
       </c>
-      <c r="V15" s="14">
+      <c r="V15" s="10">
         <v>18</v>
       </c>
-      <c r="W15" s="19">
+      <c r="W15" s="15">
         <v>0.25</v>
       </c>
-      <c r="X15" s="20"/>
-      <c r="Y15" s="12"/>
-      <c r="Z15" s="9"/>
-      <c r="AA15" s="12"/>
-      <c r="AB15" s="9"/>
-      <c r="AC15" s="80"/>
+      <c r="X15" s="16"/>
+      <c r="Y15" s="8"/>
+      <c r="Z15" s="5"/>
+      <c r="AA15" s="8"/>
+      <c r="AB15" s="5"/>
+      <c r="AC15" s="48"/>
     </row>
     <row r="16" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
+      <c r="A16" s="3">
         <v>13</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="9">
+      <c r="B16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="5">
         <v>0</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="6">
         <v>0</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="5">
         <v>0</v>
       </c>
-      <c r="F16" s="32">
+      <c r="F16" s="28">
         <v>12</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="7">
         <v>13</v>
       </c>
-      <c r="H16" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="I16" s="9">
+      <c r="H16" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I16" s="5">
         <v>49</v>
       </c>
-      <c r="J16" s="13">
+      <c r="J16" s="9">
         <v>52</v>
       </c>
-      <c r="K16" s="9">
+      <c r="K16" s="5">
         <v>52</v>
       </c>
-      <c r="L16" s="14">
+      <c r="L16" s="10">
         <v>0.5</v>
       </c>
-      <c r="M16" s="41">
+      <c r="M16" s="37">
         <f t="shared" si="0"/>
         <v>121394.23076923077</v>
       </c>
-      <c r="N16" s="15">
+      <c r="N16" s="11">
         <v>125000</v>
       </c>
-      <c r="O16" s="41">
+      <c r="O16" s="37">
         <f t="shared" si="1"/>
         <v>125000</v>
       </c>
-      <c r="P16" s="16">
+      <c r="P16" s="12">
         <v>20</v>
       </c>
-      <c r="Q16" s="17">
+      <c r="Q16" s="13">
         <v>13</v>
       </c>
-      <c r="R16" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="S16" s="14">
+      <c r="R16" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="S16" s="10">
         <v>13</v>
       </c>
-      <c r="T16" s="18">
+      <c r="T16" s="14">
         <v>14</v>
       </c>
-      <c r="U16" s="14">
+      <c r="U16" s="10">
         <v>14</v>
       </c>
-      <c r="V16" s="14">
+      <c r="V16" s="10">
         <v>20</v>
       </c>
-      <c r="W16" s="19">
+      <c r="W16" s="15">
         <v>0.05</v>
       </c>
-      <c r="X16" s="20"/>
-      <c r="Y16" s="12"/>
-      <c r="Z16" s="9"/>
-      <c r="AA16" s="12"/>
-      <c r="AB16" s="9"/>
-      <c r="AC16" s="80"/>
+      <c r="X16" s="16"/>
+      <c r="Y16" s="8"/>
+      <c r="Z16" s="5"/>
+      <c r="AA16" s="8"/>
+      <c r="AB16" s="5"/>
+      <c r="AC16" s="48"/>
     </row>
     <row r="17" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
+      <c r="A17" s="3">
         <v>14</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="9">
+      <c r="B17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="5">
         <v>241</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="6">
         <v>251</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="5">
         <v>279</v>
       </c>
-      <c r="F17" s="32">
+      <c r="F17" s="28">
         <v>6</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="7">
         <v>14</v>
       </c>
-      <c r="H17" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="I17" s="9">
+      <c r="H17" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" s="5">
         <v>42</v>
       </c>
-      <c r="J17" s="13">
+      <c r="J17" s="9">
         <v>52</v>
       </c>
-      <c r="K17" s="9">
+      <c r="K17" s="5">
         <v>55</v>
       </c>
-      <c r="L17" s="14">
+      <c r="L17" s="10">
         <v>0.5</v>
       </c>
-      <c r="M17" s="41">
+      <c r="M17" s="37">
         <f t="shared" si="0"/>
         <v>67788.461538461546</v>
       </c>
-      <c r="N17" s="15">
+      <c r="N17" s="11">
         <v>75000</v>
       </c>
-      <c r="O17" s="41">
+      <c r="O17" s="37">
         <f t="shared" si="1"/>
         <v>77163.461538461532</v>
       </c>
-      <c r="P17" s="16">
+      <c r="P17" s="12">
         <v>21</v>
       </c>
-      <c r="Q17" s="17">
+      <c r="Q17" s="13">
         <v>14</v>
       </c>
-      <c r="R17" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="S17" s="14">
+      <c r="R17" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="S17" s="10">
         <v>13</v>
       </c>
-      <c r="T17" s="18">
+      <c r="T17" s="14">
         <v>14</v>
       </c>
-      <c r="U17" s="14">
+      <c r="U17" s="10">
         <v>14</v>
       </c>
-      <c r="V17" s="14">
+      <c r="V17" s="10">
         <v>21</v>
       </c>
-      <c r="W17" s="19">
+      <c r="W17" s="15">
         <v>0.05</v>
       </c>
-      <c r="X17" s="20"/>
-      <c r="Y17" s="12"/>
-      <c r="Z17" s="9"/>
-      <c r="AA17" s="12"/>
-      <c r="AB17" s="9"/>
-      <c r="AC17" s="80"/>
+      <c r="X17" s="16"/>
+      <c r="Y17" s="8"/>
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="8"/>
+      <c r="AB17" s="5"/>
+      <c r="AC17" s="48"/>
     </row>
     <row r="18" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+      <c r="A18" s="3">
         <v>15</v>
       </c>
-      <c r="B18" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="9">
+      <c r="B18" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="5">
         <v>209</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="6">
         <v>220</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="5">
         <v>279</v>
       </c>
-      <c r="F18" s="36">
+      <c r="F18" s="32">
         <v>14</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="7">
         <v>15</v>
       </c>
-      <c r="H18" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="I18" s="9">
+      <c r="H18" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I18" s="5">
         <v>36</v>
       </c>
-      <c r="J18" s="13">
+      <c r="J18" s="9">
         <v>39</v>
       </c>
-      <c r="K18" s="9">
+      <c r="K18" s="5">
         <v>43</v>
       </c>
-      <c r="L18" s="14">
+      <c r="L18" s="10">
         <v>0.5</v>
       </c>
-      <c r="M18" s="41">
+      <c r="M18" s="37">
         <f t="shared" si="0"/>
         <v>1442307.6923076923</v>
       </c>
-      <c r="N18" s="15">
+      <c r="N18" s="11">
         <v>1500000</v>
       </c>
-      <c r="O18" s="41">
+      <c r="O18" s="37">
         <f t="shared" si="1"/>
         <v>1576923.076923077</v>
       </c>
-      <c r="P18" s="16">
+      <c r="P18" s="12">
         <v>22</v>
       </c>
-      <c r="Q18" s="17">
+      <c r="Q18" s="13">
         <v>15</v>
       </c>
-      <c r="R18" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="S18" s="14">
+      <c r="R18" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="S18" s="10">
         <v>65</v>
       </c>
-      <c r="T18" s="18">
+      <c r="T18" s="14">
         <v>70</v>
       </c>
-      <c r="U18" s="14">
+      <c r="U18" s="10">
         <v>71</v>
       </c>
-      <c r="V18" s="14">
+      <c r="V18" s="10">
         <v>22</v>
       </c>
-      <c r="W18" s="19">
+      <c r="W18" s="15">
         <v>0.02</v>
       </c>
-      <c r="X18" s="20"/>
-      <c r="Y18" s="12"/>
-      <c r="Z18" s="9"/>
-      <c r="AA18" s="12"/>
-      <c r="AB18" s="9"/>
-      <c r="AC18" s="80"/>
+      <c r="X18" s="16"/>
+      <c r="Y18" s="8"/>
+      <c r="Z18" s="5"/>
+      <c r="AA18" s="8"/>
+      <c r="AB18" s="5"/>
+      <c r="AC18" s="48"/>
     </row>
     <row r="19" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
+      <c r="A19" s="3">
         <v>16</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="9">
+      <c r="B19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="5">
         <v>667</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="6">
         <v>674</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="5">
         <v>782</v>
       </c>
-      <c r="F19" s="32">
+      <c r="F19" s="28">
         <v>14</v>
       </c>
-      <c r="G19" s="11">
+      <c r="G19" s="7">
         <v>16</v>
       </c>
-      <c r="H19" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="I19" s="9">
+      <c r="H19" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I19" s="5">
         <v>31</v>
       </c>
-      <c r="J19" s="13">
+      <c r="J19" s="9">
         <v>39</v>
       </c>
-      <c r="K19" s="9">
+      <c r="K19" s="5">
         <v>42</v>
       </c>
-      <c r="L19" s="14">
+      <c r="L19" s="10">
         <v>0.5</v>
       </c>
-      <c r="M19" s="41">
+      <c r="M19" s="37">
         <f t="shared" si="0"/>
         <v>134615.38461538462</v>
       </c>
-      <c r="N19" s="15">
+      <c r="N19" s="11">
         <v>150000</v>
       </c>
-      <c r="O19" s="41">
+      <c r="O19" s="37">
         <f t="shared" si="1"/>
         <v>155769.23076923078</v>
       </c>
-      <c r="P19" s="16">
+      <c r="P19" s="12">
         <v>23</v>
       </c>
-      <c r="Q19" s="17">
+      <c r="Q19" s="13">
         <v>16</v>
       </c>
-      <c r="R19" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="S19" s="14">
+      <c r="R19" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="S19" s="10">
         <v>25</v>
       </c>
-      <c r="T19" s="18">
+      <c r="T19" s="14">
         <v>28</v>
       </c>
-      <c r="U19" s="14">
+      <c r="U19" s="10">
         <v>32</v>
       </c>
-      <c r="V19" s="14">
+      <c r="V19" s="10">
         <v>23</v>
       </c>
-      <c r="W19" s="19">
+      <c r="W19" s="15">
         <v>0.05</v>
       </c>
-      <c r="X19" s="20"/>
-      <c r="Y19" s="12"/>
-      <c r="Z19" s="9"/>
-      <c r="AA19" s="12"/>
-      <c r="AB19" s="9"/>
-      <c r="AC19" s="80"/>
+      <c r="X19" s="16"/>
+      <c r="Y19" s="8"/>
+      <c r="Z19" s="5"/>
+      <c r="AA19" s="8"/>
+      <c r="AB19" s="5"/>
+      <c r="AC19" s="48"/>
     </row>
     <row r="20" spans="1:29" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+      <c r="A20" s="3">
         <v>17</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="9">
+      <c r="B20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="5">
         <v>0</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="6">
         <v>0</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="5">
         <v>0</v>
       </c>
-      <c r="F20" s="32">
+      <c r="F20" s="28">
         <v>16</v>
       </c>
-      <c r="G20" s="11">
+      <c r="G20" s="7">
         <v>17</v>
       </c>
-      <c r="H20" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="I20" s="9">
+      <c r="H20" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="I20" s="5">
         <v>52</v>
       </c>
-      <c r="J20" s="13">
+      <c r="J20" s="9">
         <v>52</v>
       </c>
-      <c r="K20" s="9">
+      <c r="K20" s="5">
         <v>55</v>
       </c>
-      <c r="L20" s="14">
+      <c r="L20" s="10">
         <v>0.5</v>
       </c>
-      <c r="M20" s="41">
+      <c r="M20" s="37">
         <f t="shared" si="0"/>
         <v>200000</v>
       </c>
-      <c r="N20" s="15">
+      <c r="N20" s="11">
         <v>200000</v>
       </c>
-      <c r="O20" s="41">
+      <c r="O20" s="37">
         <f t="shared" si="1"/>
         <v>205769.23076923075</v>
       </c>
-      <c r="P20" s="16">
+      <c r="P20" s="12">
         <v>26</v>
       </c>
-      <c r="Q20" s="17">
+      <c r="Q20" s="13">
         <v>17</v>
       </c>
-      <c r="R20" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="S20" s="14">
+      <c r="R20" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="S20" s="10">
         <v>39</v>
       </c>
-      <c r="T20" s="18">
+      <c r="T20" s="14">
         <v>42</v>
       </c>
-      <c r="U20" s="14">
+      <c r="U20" s="10">
         <v>47</v>
       </c>
-      <c r="V20" s="14">
+      <c r="V20" s="10">
         <v>26</v>
       </c>
-      <c r="W20" s="19">
+      <c r="W20" s="15">
         <v>0.02</v>
       </c>
-      <c r="X20" s="20"/>
-      <c r="Y20" s="12"/>
-      <c r="Z20" s="9"/>
-      <c r="AA20" s="12"/>
-      <c r="AB20" s="9"/>
-      <c r="AC20" s="80"/>
+      <c r="X20" s="16"/>
+      <c r="Y20" s="8"/>
+      <c r="Z20" s="5"/>
+      <c r="AA20" s="8"/>
+      <c r="AB20" s="5"/>
+      <c r="AC20" s="48"/>
     </row>
     <row r="21" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
+      <c r="A21" s="3">
         <v>18</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="9">
+      <c r="B21" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="5">
         <v>120</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="6">
         <v>130</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="5">
         <v>147</v>
       </c>
-      <c r="F21" s="32">
+      <c r="F21" s="28">
         <v>17</v>
       </c>
-      <c r="G21" s="11">
+      <c r="G21" s="7">
         <v>18</v>
       </c>
-      <c r="H21" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="I21" s="9">
+      <c r="H21" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I21" s="5">
         <v>22</v>
       </c>
-      <c r="J21" s="13">
+      <c r="J21" s="9">
         <v>26</v>
       </c>
-      <c r="K21" s="9">
+      <c r="K21" s="5">
         <v>27</v>
       </c>
-      <c r="L21" s="14">
+      <c r="L21" s="10">
         <v>0.5</v>
       </c>
-      <c r="M21" s="41">
+      <c r="M21" s="37">
         <f t="shared" si="0"/>
         <v>69230.769230769234</v>
       </c>
-      <c r="N21" s="15">
+      <c r="N21" s="11">
         <v>75000</v>
       </c>
-      <c r="O21" s="41">
+      <c r="O21" s="37">
         <f t="shared" si="1"/>
         <v>76442.307692307688</v>
       </c>
-      <c r="P21" s="16">
+      <c r="P21" s="12">
         <v>28</v>
       </c>
-      <c r="Q21" s="17">
+      <c r="Q21" s="13">
         <v>18</v>
       </c>
-      <c r="R21" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="S21" s="14">
+      <c r="R21" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="S21" s="10">
         <v>13</v>
       </c>
-      <c r="T21" s="18">
+      <c r="T21" s="14">
         <v>14</v>
       </c>
-      <c r="U21" s="14">
+      <c r="U21" s="10">
         <v>17</v>
       </c>
-      <c r="V21" s="14">
+      <c r="V21" s="10">
         <v>28</v>
       </c>
-      <c r="W21" s="19">
+      <c r="W21" s="15">
         <v>0.05</v>
       </c>
-      <c r="X21" s="20"/>
-      <c r="Y21" s="12"/>
-      <c r="Z21" s="9"/>
-      <c r="AA21" s="12"/>
-      <c r="AB21" s="9"/>
-      <c r="AC21" s="80"/>
+      <c r="X21" s="16"/>
+      <c r="Y21" s="8"/>
+      <c r="Z21" s="5"/>
+      <c r="AA21" s="8"/>
+      <c r="AB21" s="5"/>
+      <c r="AC21" s="48"/>
     </row>
     <row r="22" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7">
+      <c r="A22" s="3">
         <v>19</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="9">
+      <c r="B22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="5">
         <v>0</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="6">
         <v>0</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="5">
         <v>0</v>
       </c>
-      <c r="F22" s="32">
+      <c r="F22" s="28">
         <v>18</v>
       </c>
-      <c r="G22" s="22">
+      <c r="G22" s="18">
         <v>19</v>
       </c>
-      <c r="H22" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="I22" s="24">
+      <c r="H22" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="I22" s="20">
         <v>5</v>
       </c>
-      <c r="J22" s="25">
+      <c r="J22" s="21">
         <v>7</v>
       </c>
-      <c r="K22" s="24">
+      <c r="K22" s="20">
         <v>8</v>
       </c>
-      <c r="L22" s="26">
+      <c r="L22" s="22">
         <v>0.5</v>
       </c>
-      <c r="M22" s="41">
+      <c r="M22" s="37">
         <f t="shared" si="0"/>
         <v>214285.71428571429</v>
       </c>
-      <c r="N22" s="26">
+      <c r="N22" s="22">
         <v>250000</v>
       </c>
-      <c r="O22" s="41">
+      <c r="O22" s="37">
         <f t="shared" si="1"/>
         <v>267857.14285714284</v>
       </c>
-      <c r="P22" s="27">
+      <c r="P22" s="23">
         <v>30</v>
       </c>
-      <c r="Q22" s="28">
+      <c r="Q22" s="24">
         <v>19</v>
       </c>
-      <c r="R22" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="S22" s="26">
+      <c r="R22" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="S22" s="22">
         <v>130</v>
       </c>
-      <c r="T22" s="29">
+      <c r="T22" s="25">
         <v>140</v>
       </c>
-      <c r="U22" s="26">
+      <c r="U22" s="22">
         <v>160</v>
       </c>
-      <c r="V22" s="26">
+      <c r="V22" s="22">
         <v>30</v>
       </c>
-      <c r="W22" s="30">
+      <c r="W22" s="26">
         <v>0.01</v>
       </c>
-      <c r="X22" s="31"/>
-      <c r="Y22" s="23"/>
-      <c r="Z22" s="24"/>
-      <c r="AA22" s="23"/>
-      <c r="AB22" s="24"/>
-      <c r="AC22" s="81"/>
+      <c r="X22" s="27"/>
+      <c r="Y22" s="19"/>
+      <c r="Z22" s="20"/>
+      <c r="AA22" s="19"/>
+      <c r="AB22" s="20"/>
+      <c r="AC22" s="49"/>
     </row>
     <row r="23" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
+      <c r="A23" s="3">
         <v>20</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="9">
+      <c r="B23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="5">
         <v>519</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="6">
         <v>530</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="5">
         <v>620</v>
       </c>
-      <c r="F23" s="32">
+      <c r="F23" s="28">
         <v>13</v>
       </c>
-      <c r="G23" s="33"/>
-      <c r="L23" s="34"/>
-      <c r="M23" s="42"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="42"/>
-      <c r="P23" s="34"/>
-      <c r="Q23" s="34"/>
-      <c r="R23" s="34"/>
-      <c r="S23" s="34"/>
-      <c r="T23" s="34"/>
-      <c r="U23" s="34"/>
-      <c r="V23" s="34"/>
-      <c r="W23" s="34"/>
+      <c r="G23" s="29"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="38"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="38"/>
+      <c r="P23" s="30"/>
+      <c r="Q23" s="30"/>
+      <c r="R23" s="30"/>
+      <c r="S23" s="30"/>
+      <c r="T23" s="30"/>
+      <c r="U23" s="30"/>
+      <c r="V23" s="30"/>
+      <c r="W23" s="30"/>
     </row>
     <row r="24" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="7">
+      <c r="A24" s="3">
         <v>21</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="5">
+        <v>396</v>
+      </c>
+      <c r="D24" s="6">
+        <v>400</v>
+      </c>
+      <c r="E24" s="5">
+        <v>460</v>
+      </c>
+      <c r="F24" s="28">
+        <v>6</v>
+      </c>
+      <c r="G24" s="29"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="38"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="38"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="30"/>
+      <c r="R24" s="30"/>
+      <c r="S24" s="30"/>
+      <c r="T24" s="30"/>
+      <c r="U24" s="30"/>
+      <c r="V24" s="30"/>
+      <c r="W24" s="30"/>
+    </row>
+    <row r="25" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>22</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="5">
+        <v>326</v>
+      </c>
+      <c r="D25" s="6">
+        <v>340</v>
+      </c>
+      <c r="E25" s="5">
+        <v>415</v>
+      </c>
+      <c r="F25" s="28">
+        <v>6</v>
+      </c>
+      <c r="G25" s="29"/>
+      <c r="L25" s="30"/>
+      <c r="M25" s="38"/>
+      <c r="O25" s="38"/>
+      <c r="P25" s="30"/>
+      <c r="Q25" s="30"/>
+      <c r="R25" s="30"/>
+      <c r="S25" s="30"/>
+      <c r="T25" s="30"/>
+      <c r="U25" s="30"/>
+      <c r="V25" s="30"/>
+      <c r="W25" s="30"/>
+    </row>
+    <row r="26" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>23</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="5">
+        <v>856</v>
+      </c>
+      <c r="D26" s="6">
+        <v>930</v>
+      </c>
+      <c r="E26" s="5">
+        <v>1209</v>
+      </c>
+      <c r="F26" s="28">
+        <v>6</v>
+      </c>
+      <c r="G26" s="29"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="38"/>
+      <c r="O26" s="38"/>
+      <c r="P26" s="30"/>
+      <c r="Q26" s="30"/>
+      <c r="R26" s="30"/>
+      <c r="S26" s="30"/>
+      <c r="T26" s="30"/>
+      <c r="U26" s="30"/>
+      <c r="V26" s="30"/>
+      <c r="W26" s="30"/>
+    </row>
+    <row r="27" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>24</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="5">
+        <v>100</v>
+      </c>
+      <c r="D27" s="6">
+        <v>100</v>
+      </c>
+      <c r="E27" s="5">
+        <v>116</v>
+      </c>
+      <c r="F27" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" s="29"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="38"/>
+      <c r="O27" s="38"/>
+      <c r="P27" s="30"/>
+      <c r="Q27" s="30"/>
+      <c r="R27" s="30"/>
+      <c r="S27" s="30"/>
+      <c r="T27" s="30"/>
+      <c r="U27" s="30"/>
+      <c r="V27" s="30"/>
+      <c r="W27" s="30"/>
+    </row>
+    <row r="28" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
         <v>25</v>
       </c>
-      <c r="C24" s="9">
-        <v>396</v>
-      </c>
-      <c r="D24" s="10">
+      <c r="B28" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="5">
+        <v>0</v>
+      </c>
+      <c r="D28" s="6">
+        <v>0</v>
+      </c>
+      <c r="E28" s="5">
+        <v>0</v>
+      </c>
+      <c r="F28" s="28">
+        <v>24</v>
+      </c>
+      <c r="G28" s="29"/>
+      <c r="L28" s="30"/>
+      <c r="M28" s="38"/>
+      <c r="O28" s="38"/>
+      <c r="P28" s="30"/>
+      <c r="Q28" s="30"/>
+      <c r="R28" s="30"/>
+      <c r="S28" s="30"/>
+      <c r="T28" s="30"/>
+      <c r="U28" s="30"/>
+      <c r="V28" s="30"/>
+      <c r="W28" s="30"/>
+    </row>
+    <row r="29" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>26</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="5">
+        <v>380</v>
+      </c>
+      <c r="D29" s="6">
         <v>400</v>
       </c>
-      <c r="E24" s="9">
-        <v>460</v>
-      </c>
-      <c r="F24" s="32">
+      <c r="E29" s="5">
+        <v>508</v>
+      </c>
+      <c r="F29" s="28">
+        <v>25</v>
+      </c>
+      <c r="G29" s="29"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="38"/>
+      <c r="O29" s="38"/>
+      <c r="P29" s="30"/>
+      <c r="Q29" s="30"/>
+      <c r="R29" s="30"/>
+      <c r="S29" s="30"/>
+      <c r="T29" s="30"/>
+      <c r="U29" s="30"/>
+      <c r="V29" s="30"/>
+      <c r="W29" s="30"/>
+    </row>
+    <row r="30" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>27</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="5">
+        <v>0</v>
+      </c>
+      <c r="D30" s="6">
+        <v>0</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0</v>
+      </c>
+      <c r="F30" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="G24" s="33"/>
-      <c r="L24" s="34"/>
-      <c r="M24" s="42"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="42"/>
-      <c r="P24" s="34"/>
-      <c r="Q24" s="34"/>
-      <c r="R24" s="34"/>
-      <c r="S24" s="34"/>
-      <c r="T24" s="34"/>
-      <c r="U24" s="34"/>
-      <c r="V24" s="34"/>
-      <c r="W24" s="34"/>
-    </row>
-    <row r="25" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
+      <c r="G30" s="29"/>
+      <c r="L30" s="30"/>
+      <c r="M30" s="38"/>
+      <c r="O30" s="38"/>
+      <c r="P30" s="30"/>
+      <c r="Q30" s="30"/>
+      <c r="R30" s="30"/>
+      <c r="S30" s="30"/>
+      <c r="T30" s="30"/>
+      <c r="U30" s="30"/>
+      <c r="V30" s="30"/>
+      <c r="W30" s="30"/>
+    </row>
+    <row r="31" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>28</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="5">
+        <v>90</v>
+      </c>
+      <c r="D31" s="6">
+        <v>90</v>
+      </c>
+      <c r="E31" s="5">
+        <v>106</v>
+      </c>
+      <c r="F31" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" s="29"/>
+      <c r="L31" s="30"/>
+      <c r="M31" s="38"/>
+      <c r="O31" s="38"/>
+      <c r="P31" s="30"/>
+      <c r="Q31" s="30"/>
+      <c r="R31" s="30"/>
+      <c r="S31" s="30"/>
+      <c r="T31" s="30"/>
+      <c r="U31" s="30"/>
+      <c r="V31" s="30"/>
+      <c r="W31" s="30"/>
+    </row>
+    <row r="32" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>29</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="5">
+        <v>0</v>
+      </c>
+      <c r="D32" s="6">
+        <v>0</v>
+      </c>
+      <c r="E32" s="5">
+        <v>0</v>
+      </c>
+      <c r="F32" s="28">
+        <v>28</v>
+      </c>
+      <c r="G32" s="29"/>
+      <c r="L32" s="30"/>
+      <c r="M32" s="38"/>
+      <c r="O32" s="38"/>
+      <c r="P32" s="30"/>
+      <c r="Q32" s="30"/>
+      <c r="R32" s="30"/>
+      <c r="S32" s="30"/>
+      <c r="T32" s="30"/>
+      <c r="U32" s="30"/>
+      <c r="V32" s="30"/>
+      <c r="W32" s="30"/>
+    </row>
+    <row r="33" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>30</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="9">
-        <v>326</v>
-      </c>
-      <c r="D25" s="10">
-        <v>340</v>
-      </c>
-      <c r="E25" s="9">
-        <v>415</v>
-      </c>
-      <c r="F25" s="32">
-        <v>6</v>
-      </c>
-      <c r="G25" s="33"/>
-      <c r="L25" s="34"/>
-      <c r="M25" s="42"/>
-      <c r="O25" s="42"/>
-      <c r="P25" s="34"/>
-      <c r="Q25" s="34"/>
-      <c r="R25" s="34"/>
-      <c r="S25" s="34"/>
-      <c r="T25" s="34"/>
-      <c r="U25" s="34"/>
-      <c r="V25" s="34"/>
-      <c r="W25" s="34"/>
-    </row>
-    <row r="26" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="7">
+      <c r="C33" s="5">
+        <v>19</v>
+      </c>
+      <c r="D33" s="6">
+        <v>20</v>
+      </c>
+      <c r="E33" s="5">
         <v>23</v>
       </c>
-      <c r="B26" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="9">
-        <v>856</v>
-      </c>
-      <c r="D26" s="10">
-        <v>930</v>
-      </c>
-      <c r="E26" s="9">
-        <v>1209</v>
-      </c>
-      <c r="F26" s="32">
-        <v>6</v>
-      </c>
-      <c r="G26" s="33"/>
-      <c r="L26" s="34"/>
-      <c r="M26" s="42"/>
-      <c r="O26" s="42"/>
-      <c r="P26" s="34"/>
-      <c r="Q26" s="34"/>
-      <c r="R26" s="34"/>
-      <c r="S26" s="34"/>
-      <c r="T26" s="34"/>
-      <c r="U26" s="34"/>
-      <c r="V26" s="34"/>
-      <c r="W26" s="34"/>
-    </row>
-    <row r="27" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="7">
+      <c r="F33" s="28">
+        <v>29</v>
+      </c>
+      <c r="G33" s="29"/>
+      <c r="L33" s="30"/>
+      <c r="M33" s="38"/>
+      <c r="O33" s="38"/>
+      <c r="P33" s="30"/>
+      <c r="Q33" s="30"/>
+      <c r="R33" s="30"/>
+      <c r="S33" s="30"/>
+      <c r="T33" s="30"/>
+      <c r="U33" s="30"/>
+      <c r="V33" s="30"/>
+      <c r="W33" s="30"/>
+    </row>
+    <row r="34" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>31</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="5">
+        <v>57</v>
+      </c>
+      <c r="D34" s="6">
+        <v>61</v>
+      </c>
+      <c r="E34" s="5">
+        <v>71</v>
+      </c>
+      <c r="F34" s="28">
+        <v>30</v>
+      </c>
+      <c r="G34" s="29"/>
+      <c r="L34" s="30"/>
+      <c r="M34" s="38"/>
+      <c r="O34" s="38"/>
+      <c r="P34" s="30"/>
+      <c r="Q34" s="30"/>
+      <c r="R34" s="30"/>
+      <c r="S34" s="30"/>
+      <c r="T34" s="30"/>
+      <c r="U34" s="30"/>
+      <c r="V34" s="30"/>
+      <c r="W34" s="30"/>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>32</v>
+      </c>
+      <c r="B35" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" s="9">
-        <v>100</v>
-      </c>
-      <c r="D27" s="10">
-        <v>100</v>
-      </c>
-      <c r="E27" s="9">
-        <v>116</v>
-      </c>
-      <c r="F27" s="32" t="s">
+      <c r="C35" s="5">
+        <v>29</v>
+      </c>
+      <c r="D35" s="6">
+        <v>30</v>
+      </c>
+      <c r="E35" s="5">
+        <v>35</v>
+      </c>
+      <c r="F35" s="32">
+        <v>31</v>
+      </c>
+      <c r="G35" s="33"/>
+      <c r="L35" s="30"/>
+      <c r="M35" s="38"/>
+      <c r="O35" s="38"/>
+      <c r="P35" s="30"/>
+      <c r="Q35" s="30"/>
+      <c r="R35" s="30"/>
+      <c r="S35" s="30"/>
+      <c r="T35" s="30"/>
+      <c r="U35" s="30"/>
+      <c r="V35" s="30"/>
+      <c r="W35" s="30"/>
+    </row>
+    <row r="36" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>33</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="5">
+        <v>82</v>
+      </c>
+      <c r="D36" s="6">
+        <v>90</v>
+      </c>
+      <c r="E36" s="5">
+        <v>107</v>
+      </c>
+      <c r="F36" s="28">
+        <v>31</v>
+      </c>
+      <c r="G36" s="29"/>
+      <c r="L36" s="30"/>
+      <c r="M36" s="38"/>
+      <c r="O36" s="38"/>
+      <c r="P36" s="30"/>
+      <c r="Q36" s="30"/>
+      <c r="R36" s="30"/>
+      <c r="S36" s="30"/>
+      <c r="T36" s="30"/>
+      <c r="U36" s="30"/>
+      <c r="V36" s="30"/>
+      <c r="W36" s="30"/>
+    </row>
+    <row r="37" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>34</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="5">
+        <v>119</v>
+      </c>
+      <c r="D37" s="6">
+        <v>120</v>
+      </c>
+      <c r="E37" s="5">
+        <v>149</v>
+      </c>
+      <c r="F37" s="28">
+        <v>30</v>
+      </c>
+      <c r="G37" s="29"/>
+      <c r="L37" s="30"/>
+      <c r="M37" s="38"/>
+      <c r="O37" s="38"/>
+      <c r="P37" s="30"/>
+      <c r="Q37" s="30"/>
+      <c r="R37" s="30"/>
+      <c r="S37" s="30"/>
+      <c r="T37" s="30"/>
+      <c r="U37" s="30"/>
+      <c r="V37" s="30"/>
+      <c r="W37" s="30"/>
+    </row>
+    <row r="38" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>35</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" s="5">
+        <v>0</v>
+      </c>
+      <c r="D38" s="6">
+        <v>0</v>
+      </c>
+      <c r="E38" s="5">
+        <v>0</v>
+      </c>
+      <c r="F38" s="28">
+        <v>33</v>
+      </c>
+      <c r="G38" s="29"/>
+      <c r="L38" s="30"/>
+      <c r="M38" s="38"/>
+      <c r="O38" s="38"/>
+      <c r="P38" s="30"/>
+      <c r="Q38" s="30"/>
+      <c r="R38" s="30"/>
+      <c r="S38" s="30"/>
+      <c r="T38" s="30"/>
+      <c r="U38" s="30"/>
+      <c r="V38" s="30"/>
+      <c r="W38" s="30"/>
+    </row>
+    <row r="39" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>36</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" s="5">
+        <v>18</v>
+      </c>
+      <c r="D39" s="6">
+        <v>20</v>
+      </c>
+      <c r="E39" s="5">
+        <v>24</v>
+      </c>
+      <c r="F39" s="28">
+        <v>35</v>
+      </c>
+      <c r="G39" s="29"/>
+      <c r="L39" s="30"/>
+      <c r="M39" s="38"/>
+      <c r="O39" s="38"/>
+      <c r="P39" s="30"/>
+      <c r="Q39" s="30"/>
+      <c r="R39" s="30"/>
+      <c r="S39" s="30"/>
+      <c r="T39" s="30"/>
+      <c r="U39" s="30"/>
+      <c r="V39" s="30"/>
+      <c r="W39" s="30"/>
+    </row>
+    <row r="40" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="34">
         <v>37</v>
       </c>
-      <c r="G27" s="33"/>
-      <c r="L27" s="34"/>
-      <c r="M27" s="42"/>
-      <c r="O27" s="42"/>
-      <c r="P27" s="34"/>
-      <c r="Q27" s="34"/>
-      <c r="R27" s="34"/>
-      <c r="S27" s="34"/>
-      <c r="T27" s="34"/>
-      <c r="U27" s="34"/>
-      <c r="V27" s="34"/>
-      <c r="W27" s="34"/>
-    </row>
-    <row r="28" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="7">
-        <v>25</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="9">
+      <c r="B40" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" s="20">
         <v>0</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D40" s="36">
         <v>0</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E40" s="20">
         <v>0</v>
       </c>
-      <c r="F28" s="32">
-        <v>24</v>
-      </c>
-      <c r="G28" s="33"/>
-      <c r="L28" s="34"/>
-      <c r="M28" s="42"/>
-      <c r="O28" s="42"/>
-      <c r="P28" s="34"/>
-      <c r="Q28" s="34"/>
-      <c r="R28" s="34"/>
-      <c r="S28" s="34"/>
-      <c r="T28" s="34"/>
-      <c r="U28" s="34"/>
-      <c r="V28" s="34"/>
-      <c r="W28" s="34"/>
-    </row>
-    <row r="29" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="7">
-        <v>26</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29" s="9">
-        <v>380</v>
-      </c>
-      <c r="D29" s="10">
-        <v>400</v>
-      </c>
-      <c r="E29" s="9">
-        <v>508</v>
-      </c>
-      <c r="F29" s="32">
-        <v>25</v>
-      </c>
-      <c r="G29" s="33"/>
-      <c r="L29" s="34"/>
-      <c r="M29" s="42"/>
-      <c r="O29" s="42"/>
-      <c r="P29" s="34"/>
-      <c r="Q29" s="34"/>
-      <c r="R29" s="34"/>
-      <c r="S29" s="34"/>
-      <c r="T29" s="34"/>
-      <c r="U29" s="34"/>
-      <c r="V29" s="34"/>
-      <c r="W29" s="34"/>
-    </row>
-    <row r="30" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="7">
-        <v>27</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="9">
-        <v>0</v>
-      </c>
-      <c r="D30" s="10">
-        <v>0</v>
-      </c>
-      <c r="E30" s="9">
-        <v>0</v>
-      </c>
-      <c r="F30" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="G30" s="33"/>
-      <c r="L30" s="34"/>
-      <c r="M30" s="42"/>
-      <c r="O30" s="42"/>
-      <c r="P30" s="34"/>
-      <c r="Q30" s="34"/>
-      <c r="R30" s="34"/>
-      <c r="S30" s="34"/>
-      <c r="T30" s="34"/>
-      <c r="U30" s="34"/>
-      <c r="V30" s="34"/>
-      <c r="W30" s="34"/>
-    </row>
-    <row r="31" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="7">
-        <v>28</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="9">
-        <v>90</v>
-      </c>
-      <c r="D31" s="10">
-        <v>90</v>
-      </c>
-      <c r="E31" s="9">
-        <v>106</v>
-      </c>
-      <c r="F31" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="G31" s="33"/>
-      <c r="L31" s="34"/>
-      <c r="M31" s="42"/>
-      <c r="O31" s="42"/>
-      <c r="P31" s="34"/>
-      <c r="Q31" s="34"/>
-      <c r="R31" s="34"/>
-      <c r="S31" s="34"/>
-      <c r="T31" s="34"/>
-      <c r="U31" s="34"/>
-      <c r="V31" s="34"/>
-      <c r="W31" s="34"/>
-    </row>
-    <row r="32" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="7">
-        <v>29</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="9">
-        <v>0</v>
-      </c>
-      <c r="D32" s="10">
-        <v>0</v>
-      </c>
-      <c r="E32" s="9">
-        <v>0</v>
-      </c>
-      <c r="F32" s="32">
-        <v>28</v>
-      </c>
-      <c r="G32" s="33"/>
-      <c r="L32" s="34"/>
-      <c r="M32" s="42"/>
-      <c r="O32" s="42"/>
-      <c r="P32" s="34"/>
-      <c r="Q32" s="34"/>
-      <c r="R32" s="34"/>
-      <c r="S32" s="34"/>
-      <c r="T32" s="34"/>
-      <c r="U32" s="34"/>
-      <c r="V32" s="34"/>
-      <c r="W32" s="34"/>
-    </row>
-    <row r="33" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="7">
-        <v>30</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="9">
-        <v>19</v>
-      </c>
-      <c r="D33" s="10">
-        <v>20</v>
-      </c>
-      <c r="E33" s="9">
-        <v>23</v>
-      </c>
-      <c r="F33" s="32">
-        <v>29</v>
-      </c>
-      <c r="G33" s="33"/>
-      <c r="L33" s="34"/>
-      <c r="M33" s="42"/>
-      <c r="O33" s="42"/>
-      <c r="P33" s="34"/>
-      <c r="Q33" s="34"/>
-      <c r="R33" s="34"/>
-      <c r="S33" s="34"/>
-      <c r="T33" s="34"/>
-      <c r="U33" s="34"/>
-      <c r="V33" s="34"/>
-      <c r="W33" s="34"/>
-    </row>
-    <row r="34" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="7">
-        <v>31</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="9">
-        <v>57</v>
-      </c>
-      <c r="D34" s="10">
-        <v>61</v>
-      </c>
-      <c r="E34" s="9">
-        <v>71</v>
-      </c>
-      <c r="F34" s="32">
-        <v>30</v>
-      </c>
-      <c r="G34" s="33"/>
-      <c r="L34" s="34"/>
-      <c r="M34" s="42"/>
-      <c r="O34" s="42"/>
-      <c r="P34" s="34"/>
-      <c r="Q34" s="34"/>
-      <c r="R34" s="34"/>
-      <c r="S34" s="34"/>
-      <c r="T34" s="34"/>
-      <c r="U34" s="34"/>
-      <c r="V34" s="34"/>
-      <c r="W34" s="34"/>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A35" s="7">
-        <v>32</v>
-      </c>
-      <c r="B35" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="9">
-        <v>29</v>
-      </c>
-      <c r="D35" s="10">
-        <v>30</v>
-      </c>
-      <c r="E35" s="9">
-        <v>35</v>
-      </c>
-      <c r="F35" s="36">
-        <v>31</v>
-      </c>
-      <c r="G35" s="37"/>
-      <c r="L35" s="34"/>
-      <c r="M35" s="42"/>
-      <c r="O35" s="42"/>
-      <c r="P35" s="34"/>
-      <c r="Q35" s="34"/>
-      <c r="R35" s="34"/>
-      <c r="S35" s="34"/>
-      <c r="T35" s="34"/>
-      <c r="U35" s="34"/>
-      <c r="V35" s="34"/>
-      <c r="W35" s="34"/>
-    </row>
-    <row r="36" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="7">
-        <v>33</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C36" s="9">
-        <v>82</v>
-      </c>
-      <c r="D36" s="10">
-        <v>90</v>
-      </c>
-      <c r="E36" s="9">
-        <v>107</v>
-      </c>
-      <c r="F36" s="32">
-        <v>31</v>
-      </c>
-      <c r="G36" s="33"/>
-      <c r="L36" s="34"/>
-      <c r="M36" s="42"/>
-      <c r="O36" s="42"/>
-      <c r="P36" s="34"/>
-      <c r="Q36" s="34"/>
-      <c r="R36" s="34"/>
-      <c r="S36" s="34"/>
-      <c r="T36" s="34"/>
-      <c r="U36" s="34"/>
-      <c r="V36" s="34"/>
-      <c r="W36" s="34"/>
-    </row>
-    <row r="37" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="7">
-        <v>34</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37" s="9">
-        <v>119</v>
-      </c>
-      <c r="D37" s="10">
-        <v>120</v>
-      </c>
-      <c r="E37" s="9">
-        <v>149</v>
-      </c>
-      <c r="F37" s="32">
-        <v>30</v>
-      </c>
-      <c r="G37" s="33"/>
-      <c r="L37" s="34"/>
-      <c r="M37" s="42"/>
-      <c r="O37" s="42"/>
-      <c r="P37" s="34"/>
-      <c r="Q37" s="34"/>
-      <c r="R37" s="34"/>
-      <c r="S37" s="34"/>
-      <c r="T37" s="34"/>
-      <c r="U37" s="34"/>
-      <c r="V37" s="34"/>
-      <c r="W37" s="34"/>
-    </row>
-    <row r="38" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="7">
-        <v>35</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38" s="9">
-        <v>0</v>
-      </c>
-      <c r="D38" s="10">
-        <v>0</v>
-      </c>
-      <c r="E38" s="9">
-        <v>0</v>
-      </c>
-      <c r="F38" s="32">
-        <v>33</v>
-      </c>
-      <c r="G38" s="33"/>
-      <c r="L38" s="34"/>
-      <c r="M38" s="42"/>
-      <c r="O38" s="42"/>
-      <c r="P38" s="34"/>
-      <c r="Q38" s="34"/>
-      <c r="R38" s="34"/>
-      <c r="S38" s="34"/>
-      <c r="T38" s="34"/>
-      <c r="U38" s="34"/>
-      <c r="V38" s="34"/>
-      <c r="W38" s="34"/>
-    </row>
-    <row r="39" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="7">
+      <c r="F40" s="47">
         <v>36</v>
       </c>
-      <c r="B39" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C39" s="9">
-        <v>18</v>
-      </c>
-      <c r="D39" s="10">
-        <v>20</v>
-      </c>
-      <c r="E39" s="9">
-        <v>24</v>
-      </c>
-      <c r="F39" s="32">
-        <v>35</v>
-      </c>
-      <c r="G39" s="33"/>
-      <c r="L39" s="34"/>
-      <c r="M39" s="42"/>
-      <c r="O39" s="42"/>
-      <c r="P39" s="34"/>
-      <c r="Q39" s="34"/>
-      <c r="R39" s="34"/>
-      <c r="S39" s="34"/>
-      <c r="T39" s="34"/>
-      <c r="U39" s="34"/>
-      <c r="V39" s="34"/>
-      <c r="W39" s="34"/>
-    </row>
-    <row r="40" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="38">
-        <v>37</v>
-      </c>
-      <c r="B40" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" s="24">
-        <v>0</v>
-      </c>
-      <c r="D40" s="40">
-        <v>0</v>
-      </c>
-      <c r="E40" s="24">
-        <v>0</v>
-      </c>
-      <c r="F40" s="77">
-        <v>36</v>
-      </c>
-      <c r="G40" s="33"/>
-      <c r="L40" s="34"/>
-      <c r="M40" s="42"/>
-      <c r="O40" s="42"/>
-      <c r="P40" s="34"/>
-      <c r="Q40" s="34"/>
-      <c r="R40" s="34"/>
-      <c r="S40" s="34"/>
-      <c r="T40" s="34"/>
-      <c r="U40" s="34"/>
-      <c r="V40" s="34"/>
-      <c r="W40" s="34"/>
+      <c r="G40" s="29"/>
+      <c r="L40" s="30"/>
+      <c r="M40" s="38"/>
+      <c r="O40" s="38"/>
+      <c r="P40" s="30"/>
+      <c r="Q40" s="30"/>
+      <c r="R40" s="30"/>
+      <c r="S40" s="30"/>
+      <c r="T40" s="30"/>
+      <c r="U40" s="30"/>
+      <c r="V40" s="30"/>
+      <c r="W40" s="30"/>
     </row>
     <row r="41" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="65"/>
-      <c r="B41" s="66"/>
-      <c r="C41" s="67"/>
-      <c r="D41" s="68"/>
-      <c r="E41" s="67"/>
-      <c r="F41" s="65"/>
-      <c r="L41" s="34"/>
-      <c r="M41" s="42"/>
-      <c r="O41" s="42"/>
-      <c r="P41" s="34"/>
-      <c r="Q41" s="34"/>
-      <c r="R41" s="34"/>
-      <c r="S41" s="34"/>
-      <c r="T41" s="34"/>
-      <c r="U41" s="34"/>
-      <c r="V41" s="34"/>
-      <c r="W41" s="34"/>
+      <c r="A41" s="39"/>
+      <c r="B41" s="40"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="41"/>
+      <c r="F41" s="39"/>
+      <c r="L41" s="30"/>
+      <c r="M41" s="38"/>
+      <c r="O41" s="38"/>
+      <c r="P41" s="30"/>
+      <c r="Q41" s="30"/>
+      <c r="R41" s="30"/>
+      <c r="S41" s="30"/>
+      <c r="T41" s="30"/>
+      <c r="U41" s="30"/>
+      <c r="V41" s="30"/>
+      <c r="W41" s="30"/>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A42" s="65"/>
-      <c r="B42" s="65"/>
-      <c r="C42" s="65"/>
-      <c r="D42" s="65"/>
-      <c r="E42" s="65"/>
-      <c r="F42" s="65"/>
-      <c r="L42" s="34"/>
-      <c r="M42" s="42"/>
-      <c r="O42" s="42"/>
-      <c r="P42" s="34"/>
-      <c r="Q42" s="34"/>
-      <c r="R42" s="34"/>
-      <c r="S42" s="34"/>
-      <c r="T42" s="34"/>
-      <c r="U42" s="34"/>
-      <c r="V42" s="34"/>
-      <c r="W42" s="34"/>
+      <c r="A42" s="39"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="L42" s="30"/>
+      <c r="M42" s="38"/>
+      <c r="O42" s="38"/>
+      <c r="P42" s="30"/>
+      <c r="Q42" s="30"/>
+      <c r="R42" s="30"/>
+      <c r="S42" s="30"/>
+      <c r="T42" s="30"/>
+      <c r="U42" s="30"/>
+      <c r="V42" s="30"/>
+      <c r="W42" s="30"/>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="L43" s="34"/>
-      <c r="M43" s="42"/>
-      <c r="O43" s="42"/>
-      <c r="P43" s="34"/>
-      <c r="Q43" s="34"/>
-      <c r="R43" s="34"/>
-      <c r="S43" s="34"/>
-      <c r="T43" s="34"/>
-      <c r="U43" s="34"/>
-      <c r="V43" s="34"/>
-      <c r="W43" s="34"/>
+      <c r="L43" s="30"/>
+      <c r="M43" s="38"/>
+      <c r="O43" s="38"/>
+      <c r="P43" s="30"/>
+      <c r="Q43" s="30"/>
+      <c r="R43" s="30"/>
+      <c r="S43" s="30"/>
+      <c r="T43" s="30"/>
+      <c r="U43" s="30"/>
+      <c r="V43" s="30"/>
+      <c r="W43" s="30"/>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="L44" s="34"/>
-      <c r="M44" s="42"/>
-      <c r="O44" s="42"/>
-      <c r="P44" s="34"/>
-      <c r="Q44" s="34"/>
-      <c r="R44" s="34"/>
-      <c r="S44" s="34"/>
-      <c r="T44" s="34"/>
-      <c r="U44" s="34"/>
-      <c r="V44" s="34"/>
-      <c r="W44" s="34"/>
+      <c r="L44" s="30"/>
+      <c r="M44" s="38"/>
+      <c r="O44" s="38"/>
+      <c r="P44" s="30"/>
+      <c r="Q44" s="30"/>
+      <c r="R44" s="30"/>
+      <c r="S44" s="30"/>
+      <c r="T44" s="30"/>
+      <c r="U44" s="30"/>
+      <c r="V44" s="30"/>
+      <c r="W44" s="30"/>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="L45" s="34"/>
-      <c r="M45" s="42"/>
-      <c r="O45" s="42"/>
-      <c r="P45" s="34"/>
-      <c r="Q45" s="34"/>
-      <c r="R45" s="34"/>
-      <c r="S45" s="34"/>
-      <c r="T45" s="34"/>
-      <c r="U45" s="34"/>
-      <c r="V45" s="34"/>
-      <c r="W45" s="34"/>
+      <c r="L45" s="30"/>
+      <c r="M45" s="38"/>
+      <c r="O45" s="38"/>
+      <c r="P45" s="30"/>
+      <c r="Q45" s="30"/>
+      <c r="R45" s="30"/>
+      <c r="S45" s="30"/>
+      <c r="T45" s="30"/>
+      <c r="U45" s="30"/>
+      <c r="V45" s="30"/>
+      <c r="W45" s="30"/>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="L46" s="34"/>
-      <c r="M46" s="42"/>
-      <c r="O46" s="42"/>
-      <c r="P46" s="34"/>
-      <c r="Q46" s="34"/>
-      <c r="R46" s="34"/>
-      <c r="S46" s="34"/>
-      <c r="T46" s="34"/>
-      <c r="U46" s="34"/>
-      <c r="V46" s="34"/>
-      <c r="W46" s="34"/>
+      <c r="L46" s="30"/>
+      <c r="M46" s="38"/>
+      <c r="O46" s="38"/>
+      <c r="P46" s="30"/>
+      <c r="Q46" s="30"/>
+      <c r="R46" s="30"/>
+      <c r="S46" s="30"/>
+      <c r="T46" s="30"/>
+      <c r="U46" s="30"/>
+      <c r="V46" s="30"/>
+      <c r="W46" s="30"/>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="L47" s="34"/>
-      <c r="M47" s="42"/>
-      <c r="O47" s="42"/>
-      <c r="P47" s="34"/>
-      <c r="Q47" s="34"/>
-      <c r="R47" s="34"/>
-      <c r="S47" s="34"/>
-      <c r="T47" s="34"/>
-      <c r="U47" s="34"/>
-      <c r="V47" s="34"/>
-      <c r="W47" s="34"/>
+      <c r="L47" s="30"/>
+      <c r="M47" s="38"/>
+      <c r="O47" s="38"/>
+      <c r="P47" s="30"/>
+      <c r="Q47" s="30"/>
+      <c r="R47" s="30"/>
+      <c r="S47" s="30"/>
+      <c r="T47" s="30"/>
+      <c r="U47" s="30"/>
+      <c r="V47" s="30"/>
+      <c r="W47" s="30"/>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="L48" s="34"/>
-      <c r="M48" s="42"/>
-      <c r="O48" s="42"/>
-      <c r="P48" s="34"/>
-      <c r="Q48" s="34"/>
-      <c r="R48" s="34"/>
-      <c r="S48" s="34"/>
-      <c r="T48" s="34"/>
-      <c r="U48" s="34"/>
-      <c r="V48" s="34"/>
-      <c r="W48" s="34"/>
+      <c r="L48" s="30"/>
+      <c r="M48" s="38"/>
+      <c r="O48" s="38"/>
+      <c r="P48" s="30"/>
+      <c r="Q48" s="30"/>
+      <c r="R48" s="30"/>
+      <c r="S48" s="30"/>
+      <c r="T48" s="30"/>
+      <c r="U48" s="30"/>
+      <c r="V48" s="30"/>
+      <c r="W48" s="30"/>
     </row>
     <row r="49" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L49" s="34"/>
-      <c r="M49" s="42"/>
-      <c r="N49" s="34"/>
+      <c r="L49" s="30"/>
+      <c r="M49" s="38"/>
+      <c r="N49" s="30"/>
       <c r="O49" s="1"/>
     </row>
     <row r="50" spans="12:15" x14ac:dyDescent="0.25">
@@ -36683,6 +37125,12 @@
     <protectedRange sqref="J4:J22" name="Range1"/>
   </protectedRanges>
   <mergeCells count="18">
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="W2:W3"/>
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="L2:O2"/>
     <mergeCell ref="S2:U2"/>
@@ -36695,14 +37143,9 @@
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="Y2:Y3"/>
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="AC2:AC3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="W2:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>